<commit_message>
add in save_data fx
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -165,7 +165,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">quelquechose on francais - oui oui</t>
+    <t xml:space="preserve">quelque chose en francais - oui oui</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1187,7 +1187,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{008F00A8-006D-4CF0-8578-00D0004E00F9}">
+          <x14:cfRule type="duplicateValues" priority="1" id="{008500EE-0045-4C1E-A938-00E5001400C7}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -1203,7 +1203,7 @@
           <xm:sqref>A:A</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{008E00F2-00BC-47A5-8275-00E8004D0006}">
+          <x14:cfRule type="duplicateValues" priority="1" id="{00E90099-00BA-4059-AB67-000600230039}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>

</xml_diff>

<commit_message>
Edit tableoftables to reflect new fulton data
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CF8485-93F4-4AB9-B71B-C53E4FA20CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -84,7 +104,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t xml:space="preserve">acute jaundice syndrome</t>
+    <t>acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -93,13 +113,13 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{sitrep} walkthroughs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC by-NC-SA 4.0</t>
+    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+  </si>
+  <si>
+    <t>{sitrep} walkthroughs</t>
+  </si>
+  <si>
+    <t>CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -108,7 +128,7 @@
     <t>population</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -120,13 +140,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -144,7 +164,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data for a mortality survey</t>
+    <t>Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -156,7 +176,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
+    <t>Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -165,23 +185,50 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">quelque chose en francais - oui oui</t>
+    <t>quelque chose en francais - oui oui</t>
+  </si>
+  <si>
+    <t>fulton_data</t>
+  </si>
+  <si>
+    <t>fulton_data_clean</t>
+  </si>
+  <si>
+    <t>rds</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>covid-19</t>
+  </si>
+  <si>
+    <t>Jittered COVID-19 linelist data from Fulton County</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>fulton_population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">County-level population data </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -197,322 +244,62 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -715,31 +502,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="22.953125"/>
-    <col min="2" max="3" width="9.00390625"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" width="12.140625"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" width="12.08203125"/>
-    <col bestFit="1" min="8" max="8" width="10.65234375"/>
-    <col bestFit="1" min="9" max="9" width="22.61328125"/>
-    <col customWidth="1" min="10" max="12" width="11.140625"/>
-    <col bestFit="1" min="13" max="13" width="10.57421875"/>
-    <col bestFit="1" min="14" max="14" width="10.421875"/>
-    <col bestFit="1" min="16" max="16" width="39.76171875"/>
+    <col min="1" max="1" width="23" bestFit="1"/>
+    <col min="2" max="3" width="9"/>
+    <col min="4" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1"/>
+    <col min="10" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1"/>
+    <col min="16" max="16" width="39.7109375" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" customHeight="1">
+    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,20 +580,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -814,41 +602,41 @@
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
       <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>2016</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="s">
         <v>28</v>
       </c>
       <c r="P2" t="str">
-        <f t="shared" ref="P2:P8" si="0">_xlfn.CONCAT(SUBSTITUTE(I2," ",""),"_",J2,"_",G2,"_",L2)</f>
+        <f t="shared" ref="P2:P9" si="0">_xlfn.CONCAT(SUBSTITUTE(I2," ",""),"_",J2,"_",G2,"_",L2)</f>
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
-      <c r="Q2" s="2" t="str">
-        <f t="shared" ref="Q2:Q8" si="1">_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2,"_",J2,"_",L2)</f>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q10" si="1">_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2,"_",J2,"_",L2)</f>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
@@ -857,10 +645,10 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
@@ -869,19 +657,19 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>2016</v>
       </c>
       <c r="M3" t="s">
@@ -890,19 +678,19 @@
       <c r="N3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" t="s">
         <v>28</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" si="0"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
-      <c r="Q3" s="2" t="str">
+      <c r="Q3" t="str">
         <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -912,10 +700,10 @@
       <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
@@ -924,19 +712,19 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
         <v>2016</v>
       </c>
       <c r="M4" t="s">
@@ -945,74 +733,74 @@
       <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" t="s">
         <v>28</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="0"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
-      <c r="Q4" s="2" t="str">
+      <c r="Q4" t="str">
         <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>2016</v>
       </c>
       <c r="M5" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" t="s">
         <v>28</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="0"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
-      <c r="Q5" s="2" t="str">
+      <c r="Q5" t="str">
         <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1022,10 +810,10 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
@@ -1034,7 +822,7 @@
       <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
       <c r="I6" t="s">
@@ -1043,10 +831,10 @@
       <c r="J6" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>2021</v>
       </c>
       <c r="M6" t="s">
@@ -1055,19 +843,19 @@
       <c r="N6" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" t="s">
         <v>44</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="0"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
-      <c r="Q6" s="2" t="str">
+      <c r="Q6" t="str">
         <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1077,10 +865,10 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -1089,7 +877,7 @@
       <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>22</v>
       </c>
       <c r="I7" t="s">
@@ -1098,7 +886,7 @@
       <c r="J7" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" t="s">
         <v>42</v>
       </c>
       <c r="L7">
@@ -1110,44 +898,44 @@
       <c r="N7" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" t="s">
         <v>44</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="0"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
-      <c r="Q7" s="2" t="str">
+      <c r="Q7" t="str">
         <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>21</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>23</v>
       </c>
       <c r="J8" t="s">
@@ -1168,7 +956,7 @@
       <c r="O8" t="s">
         <v>28</v>
       </c>
-      <c r="P8" s="3" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="0"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
@@ -1176,50 +964,180 @@
         <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
-      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9">
+        <v>2020</v>
+      </c>
+      <c r="M9" t="s">
+        <v>56</v>
+      </c>
+      <c r="N9" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I9," ",""),"_",J9,"_",G9,"_",L9)</f>
+        <v>covid-19_outbreak_usa_2020</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="1"/>
+        <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>2020</v>
+      </c>
+      <c r="M10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <v>covid-19_outbreak_usa_2020</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="1"/>
+        <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <v>2020</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I11," ",""),"_",J11,"_",G11,"_",L11)</f>
+        <v>covid-19_outbreak_usa_2020</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" ref="Q11" si="2">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{008500EE-0045-4C1E-A938-00E5001400C7}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A:A</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{00E90099-00BA-4059-AB67-000600230039}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A8</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add mpox (R practical) rdas, edited tableoftables, and documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CF8485-93F4-4AB9-B71B-C53E4FA20CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF57AF4-F02F-4765-BD38-0F775F04AE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -213,17 +213,51 @@
   </si>
   <si>
     <t xml:space="preserve">County-level population data </t>
+  </si>
+  <si>
+    <t>mpox_linelist</t>
+  </si>
+  <si>
+    <t>mpox_aggregate_table</t>
+  </si>
+  <si>
+    <t>aggregate</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>mpox</t>
+  </si>
+  <si>
+    <t>Fictional mpox case linelist in five European countries</t>
+  </si>
+  <si>
+    <t>Fictional cumulative mpox case counts in five European countries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -254,10 +288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,8 +1162,118 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11" si="2">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q13" si="2">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12">
+        <v>2022</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I12," ",""),"_",J12,"_",G12,"_",L12)</f>
+        <v>mpox_outbreak_eee_2022</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eee_2022_linelist_1_1_outbreak_2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13">
+        <v>2022</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I13," ",""),"_",J13,"_",G13,"_",L13)</f>
+        <v>mpox_outbreak_eee_2022</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eee_2022_aggregate_1_1_outbreak_2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename doc files to match group name, move rds to extdata, change to eue, devtools::document and rebuild
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,39 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF57AF4-F02F-4765-BD38-0F775F04AE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -104,7 +84,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t>acute jaundice syndrome</t>
+    <t xml:space="preserve">acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -113,13 +93,13 @@
     <t>no</t>
   </si>
   <si>
-    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
-  </si>
-  <si>
-    <t>{sitrep} walkthroughs</t>
-  </si>
-  <si>
-    <t>CC by-NC-SA 4.0</t>
+    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{sitrep} walkthroughs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -128,7 +108,7 @@
     <t>population</t>
   </si>
   <si>
-    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -140,13 +120,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -164,7 +144,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Fake data for a mortality survey</t>
+    <t xml:space="preserve">Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -176,7 +156,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t>Fake data dictionary for a mortality survey</t>
+    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -185,30 +165,30 @@
     <t>fr</t>
   </si>
   <si>
-    <t>quelque chose en francais - oui oui</t>
+    <t xml:space="preserve">quelque chose en francais - oui oui</t>
   </si>
   <si>
     <t>fulton_data</t>
   </si>
   <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>covid-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jittered COVID-19 linelist data from Fulton County</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
     <t>fulton_data_clean</t>
   </si>
   <si>
     <t>rds</t>
   </si>
   <si>
-    <t>usa</t>
-  </si>
-  <si>
-    <t>covid-19</t>
-  </si>
-  <si>
-    <t>Jittered COVID-19 linelist data from Fulton County</t>
-  </si>
-  <si>
-    <t>training</t>
-  </si>
-  <si>
     <t>fulton_population</t>
   </si>
   <si>
@@ -218,6 +198,18 @@
     <t>mpox_linelist</t>
   </si>
   <si>
+    <t>eue</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
+    <t>mpox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictional mpox case linelist in five European countries</t>
+  </si>
+  <si>
     <t>mpox_aggregate_table</t>
   </si>
   <si>
@@ -227,42 +219,23 @@
     <t>csv</t>
   </si>
   <si>
-    <t>eee</t>
-  </si>
-  <si>
-    <t>regional</t>
-  </si>
-  <si>
-    <t>mpox</t>
-  </si>
-  <si>
-    <t>Fictional mpox case linelist in five European countries</t>
-  </si>
-  <si>
-    <t>Fictional cumulative mpox case counts in five European countries</t>
+    <t xml:space="preserve">Fictional cumulative mpox case counts in five European countries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -278,64 +251,320 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="4">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -538,32 +767,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1"/>
+    <col bestFit="1" min="1" max="1" width="23"/>
     <col min="2" max="3" width="9"/>
-    <col min="4" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1"/>
-    <col min="10" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1"/>
-    <col min="16" max="16" width="39.7109375" bestFit="1"/>
+    <col bestFit="1" customWidth="1" min="4" max="5" width="12.140625"/>
+    <col bestFit="1" min="8" max="8" width="10.7109375"/>
+    <col bestFit="1" min="9" max="9" width="22.5703125"/>
+    <col customWidth="1" min="10" max="12" width="11.140625"/>
+    <col bestFit="1" min="13" max="13" width="10.5703125"/>
+    <col bestFit="1" min="14" max="14" width="10.42578125"/>
+    <col bestFit="1" min="16" max="16" width="39.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.6" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -671,7 +898,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -726,7 +953,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -781,7 +1008,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -836,7 +1063,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -891,7 +1118,7 @@
         <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -946,7 +1173,7 @@
         <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1001,7 +1228,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1021,13 +1248,13 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
@@ -1039,16 +1266,16 @@
         <v>2020</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O9" t="s">
         <v>28</v>
       </c>
       <c r="P9" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I9," ",""),"_",J9,"_",G9,"_",L9)</f>
+        <f t="shared" si="0"/>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q9" t="str">
@@ -1056,15 +1283,15 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1076,13 +1303,13 @@
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
         <v>22</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
         <v>24</v>
@@ -1094,16 +1321,16 @@
         <v>2020</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O10" t="s">
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P13" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1111,7 +1338,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1131,13 +1358,13 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
         <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J11" t="s">
         <v>24</v>
@@ -1152,28 +1379,28 @@
         <v>59</v>
       </c>
       <c r="N11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O11" t="s">
         <v>28</v>
       </c>
       <c r="P11" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I11," ",""),"_",J11,"_",G11,"_",L11)</f>
+        <f t="shared" si="2"/>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q13" si="2">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q13" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D12">
@@ -1182,108 +1409,142 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>42</v>
       </c>
       <c r="L12">
         <v>2022</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>57</v>
+      <c r="M12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="O12" t="s">
         <v>28</v>
       </c>
       <c r="P12" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I12," ",""),"_",J12,"_",G12,"_",L12)</f>
-        <v>mpox_outbreak_eee_2022</v>
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eue_2022</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="2"/>
-        <v>mpox_outbreak_eee_2022_linelist_1_1_outbreak_2022</v>
+        <f t="shared" si="3"/>
+        <v>mpox_outbreak_eue_2022_linelist_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="L13">
         <v>2022</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>57</v>
+      <c r="N13" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="O13" t="s">
         <v>28</v>
       </c>
       <c r="P13" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I13," ",""),"_",J13,"_",G13,"_",L13)</f>
-        <v>mpox_outbreak_eee_2022</v>
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eue_2022</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="2"/>
-        <v>mpox_outbreak_eee_2022_aggregate_1_1_outbreak_2022</v>
+        <f t="shared" si="3"/>
+        <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="duplicateValues" priority="2" id="{00630082-0058-421D-A219-008800C700CB}">
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="duplicateValues" priority="1" id="{006B0081-00BC-4AE9-A423-004000AF00D5}">
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A:A</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding data for salmonella outbreak in Stegen case study
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3553397-D762-4179-82A6-5A9BD82301C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -84,7 +104,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t xml:space="preserve">acute jaundice syndrome</t>
+    <t>acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -93,13 +113,13 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{sitrep} walkthroughs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC by-NC-SA 4.0</t>
+    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+  </si>
+  <si>
+    <t>{sitrep} walkthroughs</t>
+  </si>
+  <si>
+    <t>CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -108,7 +128,7 @@
     <t>population</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -120,13 +140,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -144,7 +164,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data for a mortality survey</t>
+    <t>Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -156,7 +176,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
+    <t>Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -165,7 +185,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">quelque chose en francais - oui oui</t>
+    <t>quelque chose en francais - oui oui</t>
   </si>
   <si>
     <t>fulton_data</t>
@@ -177,7 +197,7 @@
     <t>covid-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Jittered COVID-19 linelist data from Fulton County</t>
+    <t>Jittered COVID-19 linelist data from Fulton County</t>
   </si>
   <si>
     <t>training</t>
@@ -207,7 +227,7 @@
     <t>mpox</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional mpox case linelist in five European countries</t>
+    <t>Fictional mpox case linelist in five European countries</t>
   </si>
   <si>
     <t>mpox_aggregate_table</t>
@@ -219,25 +239,45 @@
     <t>csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional cumulative mpox case counts in five European countries</t>
+    <t>Fictional cumulative mpox case counts in five European countries</t>
+  </si>
+  <si>
+    <t>stegentira_data</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>salmonella</t>
+  </si>
+  <si>
+    <t>Fictional linelist of salmonella outbreak in Stegen, Germany</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -251,320 +291,62 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -767,30 +549,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="M14" activeCellId="0" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="23"/>
+    <col min="1" max="1" width="23" bestFit="1"/>
     <col min="2" max="3" width="9"/>
-    <col bestFit="1" customWidth="1" min="4" max="5" width="12.140625"/>
-    <col bestFit="1" min="8" max="8" width="10.7109375"/>
-    <col bestFit="1" min="9" max="9" width="22.5703125"/>
-    <col customWidth="1" min="10" max="12" width="11.140625"/>
-    <col bestFit="1" min="13" max="13" width="10.5703125"/>
-    <col bestFit="1" min="14" max="14" width="10.42578125"/>
-    <col bestFit="1" min="16" max="16" width="39.7109375"/>
+    <col min="4" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1"/>
+    <col min="10" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1"/>
+    <col min="16" max="16" width="39.7109375" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1">
+    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -898,7 +682,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -953,7 +737,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1008,7 +792,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1063,7 +847,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1118,7 +902,7 @@
         <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1173,7 +957,7 @@
         <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1228,7 +1012,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1283,7 +1067,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1293,10 +1077,10 @@
       <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
@@ -1330,7 +1114,7 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P13" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P14" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1338,7 +1122,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1389,18 +1173,18 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q13" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q14" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12">
@@ -1409,31 +1193,31 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" t="s">
         <v>42</v>
       </c>
       <c r="L12">
         <v>2022</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" t="s">
         <v>55</v>
       </c>
       <c r="O12" t="s">
@@ -1448,14 +1232,14 @@
         <v>mpox_outbreak_eue_2022_linelist_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>67</v>
       </c>
       <c r="D13">
@@ -1464,31 +1248,31 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" t="s">
         <v>42</v>
       </c>
       <c r="L13">
         <v>2022</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" t="s">
         <v>55</v>
       </c>
       <c r="O13" t="s">
@@ -1503,48 +1287,69 @@
         <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
       </c>
     </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14">
+        <v>1998</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="2"/>
+        <v>salmonella_outbreak_de_1998</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="3"/>
+        <v>salmonella_outbreak_de_1998_linelist_1_1_outbreak_1998</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="2" id="{00630082-0058-421D-A219-008800C700CB}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{006B0081-00BC-4AE9-A423-004000AF00D5}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A:A</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing table for #9
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -261,10 +261,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,7 +1018,7 @@
         <v>34</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1060,7 +1059,7 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1_outbreak_2016</v>
       </c>
     </row>
     <row r="6">
@@ -1412,7 +1411,7 @@
       <c r="F12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1467,7 +1466,7 @@
       <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -1512,7 +1511,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="2" id="{00630082-0058-421D-A219-008800C700CB}">
+          <x14:cfRule type="duplicateValues" priority="2" id="{00650074-000F-4D28-8BE5-00F4004F0004}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -1528,7 +1527,7 @@
           <xm:sqref>A8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{006B0081-00BC-4AE9-A423-004000AF00D5}">
+          <x14:cfRule type="duplicateValues" priority="1" id="{00180092-00BD-4131-994C-00F6006E00E2}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>

</xml_diff>

<commit_message>
Revert back to old table to prevent conflict
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3553397-D762-4179-82A6-5A9BD82301C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C8C1477-7FB6-4BFF-8845-018432AD30F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -240,36 +240,17 @@
   </si>
   <si>
     <t>Fictional cumulative mpox case counts in five European countries</t>
-  </si>
-  <si>
-    <t>stegentira_data</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>salmonella</t>
-  </si>
-  <si>
-    <t>Fictional linelist of salmonella outbreak in Stegen, Germany</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -301,9 +282,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -555,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +783,7 @@
         <v>34</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -844,7 +824,7 @@
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1_outbreak_2016</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1114,7 +1094,7 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P14" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P13" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1173,7 +1153,7 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q14" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q13" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
@@ -1285,61 +1265,6 @@
       <c r="Q13" t="str">
         <f t="shared" si="3"/>
         <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14">
-        <v>1998</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O14" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" t="str">
-        <f t="shared" si="2"/>
-        <v>salmonella_outbreak_de_1998</v>
-      </c>
-      <c r="Q14" t="str">
-        <f t="shared" si="3"/>
-        <v>salmonella_outbreak_de_1998_linelist_1_1_outbreak_1998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
linelist_cleaned rename for #22
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>name</t>
   </si>
@@ -267,10 +267,16 @@
     <t xml:space="preserve">Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
-    <t>linelist_cleaned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>linelist_cleaned_excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+  </si>
+  <si>
+    <t>linelist_cleaned_rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
 </sst>
 </file>
@@ -823,7 +829,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1779,7 +1785,7 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -1815,7 +1821,7 @@
         <v>2014</v>
       </c>
       <c r="M18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N18" t="s">
         <v>78</v>
@@ -1841,7 +1847,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{006300C6-00F7-4EC6-B572-007F000100A4}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{008100A4-0027-4C1C-94FB-001B006E0066}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -1857,7 +1863,7 @@
           <xm:sqref>A:A</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00AD00F3-008A-4A6E-9771-0042001C00E0}">
+          <x14:cfRule type="expression" priority="1" id="{00960035-000B-4110-8114-005200FF0063}">
             <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>

<commit_message>
adding malaria aggregate counts
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>name</t>
   </si>
@@ -345,19 +345,25 @@
     <t>contacts_clean</t>
   </si>
   <si>
-    <t>gpl4</t>
-  </si>
-  <si>
     <t>followups_clean</t>
   </si>
   <si>
-    <t>gpl5</t>
-  </si>
-  <si>
     <t>relationships_clean</t>
   </si>
   <si>
-    <t>gpl6</t>
+    <t>district_weekly_count_data</t>
+  </si>
+  <si>
+    <t>moz</t>
+  </si>
+  <si>
+    <t>malaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictional counts of malaria cases from Mozambique</t>
+  </si>
+  <si>
+    <t>malaria_facility_count_data</t>
   </si>
 </sst>
 </file>
@@ -921,7 +927,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="O18" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="N19" zoomScale="100" workbookViewId="0">
       <selection activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2524,7 +2530,7 @@
         <v>78</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="P29" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(I29," ",""),"_",J29,"_",G29,"_",L29)</f>
@@ -2537,7 +2543,7 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>18</v>
@@ -2579,7 +2585,7 @@
         <v>78</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="P30" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(I30," ",""),"_",J30,"_",G30,"_",L30)</f>
@@ -2592,7 +2598,7 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>18</v>
@@ -2634,7 +2640,7 @@
         <v>78</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="P31" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(I31," ",""),"_",J31,"_",G31,"_",L31)</f>
@@ -2643,6 +2649,116 @@
       <c r="Q31" t="str">
         <f>_xlfn.CONCAT(P31,"_",B31,"_",D31,"_",E31,"_",J31,"_",L31)</f>
         <v>contacttracing_outbreak_zzz_2020_linelist_4_1_outbreak_2020</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" t="s">
+        <v>114</v>
+      </c>
+      <c r="J32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32">
+        <v>2019</v>
+      </c>
+      <c r="M32" t="s">
+        <v>115</v>
+      </c>
+      <c r="N32" t="s">
+        <v>78</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P32" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I32," ",""),"_",J32,"_",G32,"_",L32)</f>
+        <v>malaria_outbreak_moz_2019</v>
+      </c>
+      <c r="Q32" t="str">
+        <f>_xlfn.CONCAT(P32,"_",B32,"_",D32,"_",E32,"_",J32,"_",L32)</f>
+        <v>malaria_outbreak_moz_2019_aggregate_1_1_outbreak_2019</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" t="s">
+        <v>114</v>
+      </c>
+      <c r="J33" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33">
+        <v>2019</v>
+      </c>
+      <c r="M33" t="s">
+        <v>115</v>
+      </c>
+      <c r="N33" t="s">
+        <v>78</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P33" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I33," ",""),"_",J33,"_",G33,"_",L33)</f>
+        <v>malaria_outbreak_moz_2019</v>
+      </c>
+      <c r="Q33" t="str">
+        <f>_xlfn.CONCAT(P33,"_",B33,"_",D33,"_",E33,"_",J33,"_",L33)</f>
+        <v>malaria_outbreak_moz_2019_aggregate_1_2_outbreak_2019</v>
       </c>
     </row>
   </sheetData>
@@ -2654,7 +2770,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{00B9005A-00ED-4050-9BF8-000D00BC0000}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{0084000C-00AE-4DB5-AA61-00D200B500CC}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2670,7 +2786,7 @@
           <xm:sqref>A:A</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{00200035-00CF-4521-9DF0-009800360058}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{00BB0084-0010-4402-88BE-002700800010}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2686,7 +2802,7 @@
           <xm:sqref>A25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00440009-0085-4ED7-A78E-00B700E500B5}">
+          <x14:cfRule type="expression" priority="1" id="{00D20029-0020-4182-BC3C-00D3002A000C}">
             <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>

<commit_message>
dont think any changes
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -485,12 +485,10 @@
     </font>
     <font>
       <sz val="11.500000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -514,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -526,9 +524,6 @@
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,7 +1032,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="M33" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="L32" zoomScale="100" workbookViewId="0">
       <selection activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1598,7 +1593,7 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P14" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P47" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1657,7 +1652,7 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q14" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q47" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
@@ -1873,11 +1868,11 @@
         <v>79</v>
       </c>
       <c r="P15" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I15," ",""),"_",J15,"_",G15,"_",L15)</f>
+        <f t="shared" si="2"/>
         <v>influenza_outbreak_chn_2013</v>
       </c>
       <c r="Q15" t="str">
-        <f>_xlfn.CONCAT(P15,"_",B15,"_",D15,"_",E15,"_",J15,"_",L15)</f>
+        <f t="shared" si="3"/>
         <v>influenza_outbreak_chn_2013_linelist_1_1_outbreak_2013</v>
       </c>
     </row>
@@ -1928,11 +1923,11 @@
         <v>79</v>
       </c>
       <c r="P16" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I16," ",""),"_",J16,"_",G16,"_",L16)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q16" t="str">
-        <f>_xlfn.CONCAT(P16,"_",B16,"_",D16,"_",E16,"_",J16,"_",L16)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_linelist_1_1_outbreak_2014</v>
       </c>
     </row>
@@ -1983,11 +1978,11 @@
         <v>79</v>
       </c>
       <c r="P17" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I17," ",""),"_",J17,"_",G17,"_",L17)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q17" t="str">
-        <f>_xlfn.CONCAT(P17,"_",B17,"_",D17,"_",E17,"_",J17,"_",L17)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_linelist_1_2_outbreak_2014</v>
       </c>
     </row>
@@ -2038,11 +2033,11 @@
         <v>79</v>
       </c>
       <c r="P18" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I18," ",""),"_",J18,"_",G18,"_",L18)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q18" t="str">
-        <f>_xlfn.CONCAT(P18,"_",B18,"_",D18,"_",E18,"_",J18,"_",L18)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_linelist_1_3_outbreak_2014</v>
       </c>
     </row>
@@ -2093,11 +2088,11 @@
         <v>79</v>
       </c>
       <c r="P19" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I19," ",""),"_",J19,"_",G19,"_",L19)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q19" t="str">
-        <f>_xlfn.CONCAT(P19,"_",B19,"_",D19,"_",E19,"_",J19,"_",L19)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_linelist_1_4_outbreak_2014</v>
       </c>
     </row>
@@ -2148,11 +2143,11 @@
         <v>79</v>
       </c>
       <c r="P20" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I20," ",""),"_",J20,"_",G20,"_",L20)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q20" t="str">
-        <f>_xlfn.CONCAT(P20,"_",B20,"_",D20,"_",E20,"_",J20,"_",L20)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_linelist_1_5_outbreak_2014</v>
       </c>
     </row>
@@ -2203,11 +2198,11 @@
         <v>79</v>
       </c>
       <c r="P21" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I21," ",""),"_",J21,"_",G21,"_",L21)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q21" t="str">
-        <f>_xlfn.CONCAT(P21,"_",B21,"_",D21,"_",E21,"_",J21,"_",L21)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_dictionary_1_1_outbreak_2014</v>
       </c>
     </row>
@@ -2258,11 +2253,11 @@
         <v>96</v>
       </c>
       <c r="P22" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I22," ",""),"_",J22,"_",G22,"_",L22)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q22" t="str">
-        <f>_xlfn.CONCAT(P22,"_",B22,"_",D22,"_",E22,"_",J22,"_",L22)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_shape_1_1_outbreak_2014</v>
       </c>
     </row>
@@ -2313,11 +2308,11 @@
         <v>96</v>
       </c>
       <c r="P23" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I23," ",""),"_",J23,"_",G23,"_",L23)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2020</v>
       </c>
       <c r="Q23" t="str">
-        <f>_xlfn.CONCAT(P23,"_",B23,"_",D23,"_",E23,"_",J23,"_",L23)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
@@ -2368,11 +2363,11 @@
         <v>79</v>
       </c>
       <c r="P24" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I24," ",""),"_",J24,"_",G24,"_",L24)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q24" t="str">
-        <f>_xlfn.CONCAT(P24,"_",B24,"_",D24,"_",E24,"_",J24,"_",L24)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_other_1_1_outbreak_2014</v>
       </c>
     </row>
@@ -2423,11 +2418,11 @@
         <v>79</v>
       </c>
       <c r="P25" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I25," ",""),"_",J25,"_",G25,"_",L25)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q25" t="str">
-        <f>_xlfn.CONCAT(P25,"_",B25,"_",D25,"_",E25,"_",J25,"_",L25)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_other_2_1_outbreak_2014</v>
       </c>
     </row>
@@ -2478,11 +2473,11 @@
         <v>79</v>
       </c>
       <c r="P26" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I26," ",""),"_",J26,"_",G26,"_",L26)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q26" t="str">
-        <f>_xlfn.CONCAT(P26,"_",B26,"_",D26,"_",E26,"_",J26,"_",L26)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_other_3_1_outbreak_2014</v>
       </c>
     </row>
@@ -2533,11 +2528,11 @@
         <v>79</v>
       </c>
       <c r="P27" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I27," ",""),"_",J27,"_",G27,"_",L27)</f>
+        <f t="shared" si="2"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q27" t="str">
-        <f>_xlfn.CONCAT(P27,"_",B27,"_",D27,"_",E27,"_",J27,"_",L27)</f>
+        <f t="shared" si="3"/>
         <v>ebola_outbreak_sle_2014_other_4_1_outbreak_2014</v>
       </c>
     </row>
@@ -2588,11 +2583,11 @@
         <v>44</v>
       </c>
       <c r="P28" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I28," ",""),"_",J28,"_",G28,"_",L28)</f>
+        <f t="shared" si="2"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q28" t="str">
-        <f>_xlfn.CONCAT(P28,"_",B28,"_",D28,"_",E28,"_",J28,"_",L28)</f>
+        <f t="shared" si="3"/>
         <v>contacttracing_outbreak_zzz_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
@@ -2643,11 +2638,11 @@
         <v>44</v>
       </c>
       <c r="P29" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I29," ",""),"_",J29,"_",G29,"_",L29)</f>
+        <f t="shared" si="2"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q29" t="str">
-        <f>_xlfn.CONCAT(P29,"_",B29,"_",D29,"_",E29,"_",J29,"_",L29)</f>
+        <f t="shared" si="3"/>
         <v>contacttracing_outbreak_zzz_2020_linelist_2_1_outbreak_2020</v>
       </c>
     </row>
@@ -2698,11 +2693,11 @@
         <v>44</v>
       </c>
       <c r="P30" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I30," ",""),"_",J30,"_",G30,"_",L30)</f>
+        <f t="shared" si="2"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q30" t="str">
-        <f>_xlfn.CONCAT(P30,"_",B30,"_",D30,"_",E30,"_",J30,"_",L30)</f>
+        <f t="shared" si="3"/>
         <v>contacttracing_outbreak_zzz_2020_linelist_3_1_outbreak_2020</v>
       </c>
     </row>
@@ -2753,11 +2748,11 @@
         <v>44</v>
       </c>
       <c r="P31" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I31," ",""),"_",J31,"_",G31,"_",L31)</f>
+        <f t="shared" si="2"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q31" t="str">
-        <f>_xlfn.CONCAT(P31,"_",B31,"_",D31,"_",E31,"_",J31,"_",L31)</f>
+        <f t="shared" si="3"/>
         <v>contacttracing_outbreak_zzz_2020_linelist_4_1_outbreak_2020</v>
       </c>
     </row>
@@ -2808,11 +2803,11 @@
         <v>28</v>
       </c>
       <c r="P32" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I32," ",""),"_",J32,"_",G32,"_",L32)</f>
+        <f t="shared" si="2"/>
         <v>malaria_outbreak_moz_2019</v>
       </c>
       <c r="Q32" t="str">
-        <f>_xlfn.CONCAT(P32,"_",B32,"_",D32,"_",E32,"_",J32,"_",L32)</f>
+        <f t="shared" si="3"/>
         <v>malaria_outbreak_moz_2019_aggregate_1_1_outbreak_2019</v>
       </c>
     </row>
@@ -2863,11 +2858,11 @@
         <v>28</v>
       </c>
       <c r="P33" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I33," ",""),"_",J33,"_",G33,"_",L33)</f>
+        <f t="shared" si="2"/>
         <v>malaria_outbreak_moz_2019</v>
       </c>
       <c r="Q33" t="str">
-        <f>_xlfn.CONCAT(P33,"_",B33,"_",D33,"_",E33,"_",J33,"_",L33)</f>
+        <f t="shared" si="3"/>
         <v>malaria_outbreak_moz_2019_aggregate_1_2_outbreak_2019</v>
       </c>
     </row>
@@ -2918,11 +2913,11 @@
         <v>28</v>
       </c>
       <c r="P34" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I34," ",""),"_",J34,"_",G34,"_",L34)</f>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q34" t="str">
-        <f>_xlfn.CONCAT(P34,"_",B34,"_",D34,"_",E34,"_",J34,"_",L34)</f>
+        <f t="shared" si="3"/>
         <v>shigella_surveillance_bel_2013_sequencing_1_1_surveillance_2013</v>
       </c>
     </row>
@@ -2973,11 +2968,11 @@
         <v>28</v>
       </c>
       <c r="P35" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I35," ",""),"_",J35,"_",G35,"_",L35)</f>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q35" t="str">
-        <f>_xlfn.CONCAT(P35,"_",B35,"_",D35,"_",E35,"_",J35,"_",L35)</f>
+        <f t="shared" si="3"/>
         <v>shigella_surveillance_bel_2013_linelist_1_1_surveillance_2013</v>
       </c>
     </row>
@@ -3028,11 +3023,11 @@
         <v>28</v>
       </c>
       <c r="P36" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I36," ",""),"_",J36,"_",G36,"_",L36)</f>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q36" t="str">
-        <f>_xlfn.CONCAT(P36,"_",B36,"_",D36,"_",E36,"_",J36,"_",L36)</f>
+        <f t="shared" si="3"/>
         <v>shigella_surveillance_bel_2013_sequencing_1_2_surveillance_2013</v>
       </c>
     </row>
@@ -3083,11 +3078,11 @@
         <v>28</v>
       </c>
       <c r="P37" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I37," ",""),"_",J37,"_",G37,"_",L37)</f>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q37" t="str">
-        <f>_xlfn.CONCAT(P37,"_",B37,"_",D37,"_",E37,"_",J37,"_",L37)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_1_1_surveillance_2020</v>
       </c>
     </row>
@@ -3138,11 +3133,11 @@
         <v>28</v>
       </c>
       <c r="P38" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I38," ",""),"_",J38,"_",G38,"_",L38)</f>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q38" t="str">
-        <f>_xlfn.CONCAT(P38,"_",B38,"_",D38,"_",E38,"_",J38,"_",L38)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_2_1_surveillance_2020</v>
       </c>
     </row>
@@ -3193,11 +3188,11 @@
         <v>28</v>
       </c>
       <c r="P39" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I39," ",""),"_",J39,"_",G39,"_",L39)</f>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q39" t="str">
-        <f>_xlfn.CONCAT(P39,"_",B39,"_",D39,"_",E39,"_",J39,"_",L39)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_3_1_surveillance_2020</v>
       </c>
     </row>
@@ -3248,11 +3243,11 @@
         <v>28</v>
       </c>
       <c r="P40" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I40," ",""),"_",J40,"_",G40,"_",L40)</f>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q40" t="str">
-        <f>_xlfn.CONCAT(P40,"_",B40,"_",D40,"_",E40,"_",J40,"_",L40)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_4_1_surveillance_2020</v>
       </c>
     </row>
@@ -3299,15 +3294,15 @@
       <c r="N41" t="s">
         <v>78</v>
       </c>
-      <c r="O41" s="6" t="s">
+      <c r="O41" s="4" t="s">
         <v>135</v>
       </c>
       <c r="P41" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I41," ",""),"_",J41,"_",G41,"_",L41)</f>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q41" t="str">
-        <f>_xlfn.CONCAT(P41,"_",B41,"_",D41,"_",E41,"_",J41,"_",L41)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_5_1_surveillance_2020</v>
       </c>
     </row>
@@ -3358,11 +3353,11 @@
         <v>28</v>
       </c>
       <c r="P42" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I42," ",""),"_",J42,"_",G42,"_",L42)</f>
+        <f t="shared" si="2"/>
         <v>likert_other_zzz_2020</v>
       </c>
       <c r="Q42" t="str">
-        <f>_xlfn.CONCAT(P42,"_",B42,"_",D42,"_",E42,"_",J42,"_",L42)</f>
+        <f t="shared" si="3"/>
         <v>likert_other_zzz_2020_aggregate_1_1_other_2020</v>
       </c>
     </row>
@@ -3403,7 +3398,7 @@
       <c r="L43">
         <v>2021</v>
       </c>
-      <c r="M43" s="6" t="s">
+      <c r="M43" s="4" t="s">
         <v>140</v>
       </c>
       <c r="N43" t="s">
@@ -3413,11 +3408,11 @@
         <v>44</v>
       </c>
       <c r="P43" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I43," ",""),"_",J43,"_",G43,"_",L43)</f>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q43" t="str">
-        <f>_xlfn.CONCAT(P43,"_",B43,"_",D43,"_",E43,"_",J43,"_",L43)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_survey_2_1_survey_2021</v>
       </c>
     </row>
@@ -3458,7 +3453,7 @@
       <c r="L44">
         <v>2021</v>
       </c>
-      <c r="M44" s="6" t="s">
+      <c r="M44" s="4" t="s">
         <v>142</v>
       </c>
       <c r="N44" t="s">
@@ -3468,11 +3463,11 @@
         <v>44</v>
       </c>
       <c r="P44" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I44," ",""),"_",J44,"_",G44,"_",L44)</f>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q44" t="str">
-        <f>_xlfn.CONCAT(P44,"_",B44,"_",D44,"_",E44,"_",J44,"_",L44)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_dictionary_2_1_survey_2021</v>
       </c>
     </row>
@@ -3513,7 +3508,7 @@
       <c r="L45">
         <v>2021</v>
       </c>
-      <c r="M45" s="6" t="s">
+      <c r="M45" s="4" t="s">
         <v>143</v>
       </c>
       <c r="N45" t="s">
@@ -3523,11 +3518,11 @@
         <v>44</v>
       </c>
       <c r="P45" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I45," ",""),"_",J45,"_",G45,"_",L45)</f>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q45" t="str">
-        <f>_xlfn.CONCAT(P45,"_",B45,"_",D45,"_",E45,"_",J45,"_",L45)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_population_1_1_survey_2021</v>
       </c>
     </row>
@@ -3578,11 +3573,11 @@
         <v>44</v>
       </c>
       <c r="P46" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I46," ",""),"_",J46,"_",G46,"_",L46)</f>
+        <f t="shared" si="2"/>
         <v>campylobacter_surveillance_deu_2001</v>
       </c>
       <c r="Q46" t="str">
-        <f>_xlfn.CONCAT(P46,"_",B46,"_",D46,"_",E46,"_",J46,"_",L46)</f>
+        <f t="shared" si="3"/>
         <v>campylobacter_surveillance_deu_2001_linelist_1_1_surveillance_2001</v>
       </c>
     </row>
@@ -3633,11 +3628,11 @@
         <v>44</v>
       </c>
       <c r="P47" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I47," ",""),"_",J47,"_",G47,"_",L47)</f>
+        <f t="shared" si="2"/>
         <v>weather_other_deu_2001</v>
       </c>
       <c r="Q47" t="str">
-        <f>_xlfn.CONCAT(P47,"_",B47,"_",D47,"_",E47,"_",J47,"_",L47)</f>
+        <f t="shared" si="3"/>
         <v>weather_other_deu_2001_aggregate_1_1_other_2001</v>
       </c>
     </row>
@@ -3650,7 +3645,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{003B00E7-0007-4FEF-AE30-00D000D800ED}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{0055004F-0014-45DA-83AE-00F000D100EE}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -3666,7 +3661,7 @@
           <xm:sqref>A:A</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{000E0081-00B4-4D23-9A96-002200F90015}">
+          <x14:cfRule type="duplicateValues" priority="3" id="{009200FD-0052-46AC-BD0D-005200B000CF}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -3682,7 +3677,7 @@
           <xm:sqref>A25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00A9004E-00B6-4F52-9784-00530022003C}">
+          <x14:cfRule type="expression" priority="1" id="{00AE00D8-0093-4F3E-B507-0037005F00C1}">
             <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>

<commit_message>
Two new datasets for case study - one on tests and one on diseases
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C7AF66-C18A-4265-A9C2-933DB5079A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="10680" yWindow="0" windowWidth="12312" windowHeight="12318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="157">
   <si>
     <t>name</t>
   </si>
@@ -84,7 +104,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t xml:space="preserve">acute jaundice syndrome</t>
+    <t>acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -93,13 +113,13 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
   </si>
   <si>
     <t>sitrep_walkthroughs</t>
   </si>
   <si>
-    <t xml:space="preserve">CC by-NC-SA 4.0</t>
+    <t>CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -108,7 +128,7 @@
     <t>population</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -120,13 +140,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -144,7 +164,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data for a mortality survey</t>
+    <t>Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -156,7 +176,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
+    <t>Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -165,7 +185,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">quelque chose en francais - oui oui</t>
+    <t>quelque chose en francais - oui oui</t>
   </si>
   <si>
     <t>fulton_data</t>
@@ -177,7 +197,7 @@
     <t>covid-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Jittered COVID-19 linelist data from Fulton County</t>
+    <t>Jittered COVID-19 linelist data from Fulton County</t>
   </si>
   <si>
     <t>case_studies</t>
@@ -207,7 +227,7 @@
     <t>mpox</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional mpox case linelist in five European countries</t>
+    <t>Fictional mpox case linelist in five European countries</t>
   </si>
   <si>
     <t>mpox_aggregate_table</t>
@@ -219,7 +239,7 @@
     <t>csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional cumulative mpox case counts in five European countries</t>
+    <t>Fictional cumulative mpox case counts in five European countries</t>
   </si>
   <si>
     <t>stegentira_data</t>
@@ -231,7 +251,7 @@
     <t>salmonella</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional linelist of salmonella outbreak in Stegen, Germany</t>
+    <t>Fictional linelist of salmonella outbreak in Stegen, Germany</t>
   </si>
   <si>
     <t>fluH7N9_China_2013</t>
@@ -246,7 +266,7 @@
     <t>influenza</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
+    <t>Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
   </si>
   <si>
     <t>epirhandbook</t>
@@ -264,52 +284,52 @@
     <t>ebola</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_excel</t>
   </si>
   <si>
-    <t xml:space="preserve">Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_rds</t>
   </si>
   <si>
-    <t xml:space="preserve">R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>hospital_linelists</t>
   </si>
   <si>
-    <t xml:space="preserve">Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_with_adm3</t>
   </si>
   <si>
-    <t xml:space="preserve">Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>cleaning_dict</t>
   </si>
   <si>
-    <t xml:space="preserve">Short example cleaning dictionary for the raw linelist</t>
+    <t>Short example cleaning dictionary for the raw linelist</t>
   </si>
   <si>
     <t>sle_adm3</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC by-IGO</t>
+    <t>Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
+  </si>
+  <si>
+    <t>CC by-IGO</t>
   </si>
   <si>
     <t>sle_admpop_adm3_2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
+    <t>Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
   </si>
   <si>
     <t>epinow_res</t>
@@ -318,7 +338,7 @@
     <t>other</t>
   </si>
   <si>
-    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>epinow_res_small</t>
@@ -327,7 +347,7 @@
     <t>generation_time</t>
   </si>
   <si>
-    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
+    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
   </si>
   <si>
     <t>incubation_period</t>
@@ -336,10 +356,10 @@
     <t>cases_clean</t>
   </si>
   <si>
-    <t xml:space="preserve">contact tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictional case data for a generic disease to demonstrate contact tracing</t>
+    <t>contact tracing</t>
+  </si>
+  <si>
+    <t>Fictional case data for a generic disease to demonstrate contact tracing</t>
   </si>
   <si>
     <t>contacts_clean</t>
@@ -360,7 +380,7 @@
     <t>malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional counts of malaria cases from Mozambique</t>
+    <t>Fictional counts of malaria cases from Mozambique</t>
   </si>
   <si>
     <t>malaria_facility_count_data</t>
@@ -384,25 +404,25 @@
     <t>surveillance</t>
   </si>
   <si>
-    <t xml:space="preserve">Next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t>Next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>sample_data_Shigella_tree</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
+    <t>Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
   </si>
   <si>
     <t>Shigella_subtree_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t>Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>country_demographics</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional country demographic and mortality data to demonstrate standardisation</t>
+    <t>Fictional country demographic and mortality data to demonstrate standardisation</t>
   </si>
   <si>
     <t>country_demographics_2</t>
@@ -417,7 +437,7 @@
     <t>world_standard_population_by_sex</t>
   </si>
   <si>
-    <t xml:space="preserve">World “standard population” by sex</t>
+    <t>World “standard population” by sex</t>
   </si>
   <si>
     <t>OGL</t>
@@ -429,22 +449,22 @@
     <t>likert</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional likert data for demonstration purposes</t>
+    <t>Fictional likert data for demonstration purposes</t>
   </si>
   <si>
     <t>survey_data</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional data for a mortality survey</t>
+    <t>Fictional data for a mortality survey</t>
   </si>
   <si>
     <t>survey_dict</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional data dictionary for a mortality survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictional population data for a mortality survey</t>
+    <t>Fictional data dictionary for a mortality survey</t>
+  </si>
+  <si>
+    <t>Fictional population data for a mortality survey</t>
   </si>
   <si>
     <t>campylobacter_germany</t>
@@ -453,7 +473,7 @@
     <t>campylobacter</t>
   </si>
   <si>
-    <t xml:space="preserve">Campylobacter surveillance data from Germany</t>
+    <t>Campylobacter surveillance data from Germany</t>
   </si>
   <si>
     <t>germany_weather</t>
@@ -462,34 +482,65 @@
     <t>weather</t>
   </si>
   <si>
-    <t xml:space="preserve">Weather data for Germany from 2001-2011</t>
+    <t>Weather data for Germany from 2001-2011</t>
+  </si>
+  <si>
+    <t>Test results for notifiable diseases reported in Feveria in 2024</t>
+  </si>
+  <si>
+    <t>Notifiable disease surveillance data in Feveria in 2024</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>notifications</t>
+  </si>
+  <si>
+    <t>multidisease_tests</t>
+  </si>
+  <si>
+    <t>multidisease_notifications</t>
+  </si>
+  <si>
+    <t>multidisease</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.500000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.000000"/>
+      <sz val="11.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -502,328 +553,76 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="2"/>
+          <bgColor indexed="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -1026,34 +825,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="L32" zoomScale="100" workbookViewId="0">
-      <selection activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="Q30" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="24.6640625"/>
-    <col customWidth="1" min="2" max="2" width="10.28125"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1"/>
+    <col min="2" max="2" width="10.26171875" customWidth="1"/>
     <col min="3" max="3" width="9"/>
-    <col bestFit="1" customWidth="1" min="4" max="5" width="12.140625"/>
-    <col bestFit="1" min="8" max="8" width="10.7109375"/>
-    <col bestFit="1" min="9" max="9" width="22.5703125"/>
-    <col customWidth="1" min="10" max="11" width="11.140625"/>
-    <col customWidth="1" min="12" max="12" width="5.7109375"/>
-    <col bestFit="1" min="13" max="13" width="10.5703125"/>
-    <col bestFit="1" min="14" max="14" width="18.140625"/>
-    <col bestFit="1" min="15" max="15" width="14.33203125"/>
-    <col bestFit="1" min="16" max="16" width="39.7109375"/>
-    <col bestFit="1" min="17" max="17" width="67.421875"/>
+    <col min="4" max="5" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.68359375" bestFit="1"/>
+    <col min="9" max="9" width="22.578125" bestFit="1"/>
+    <col min="10" max="11" width="11.15625" customWidth="1"/>
+    <col min="12" max="12" width="5.68359375" customWidth="1"/>
+    <col min="13" max="13" width="10.578125" bestFit="1"/>
+    <col min="14" max="14" width="18.15625" bestFit="1"/>
+    <col min="15" max="15" width="14.3125" bestFit="1"/>
+    <col min="16" max="16" width="39.68359375" bestFit="1"/>
+    <col min="17" max="17" width="67.41796875" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1">
+    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1161,7 +962,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1201,7 +1002,7 @@
       <c r="M3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
         <v>27</v>
       </c>
       <c r="O3" t="s">
@@ -1216,7 +1017,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1256,7 +1057,7 @@
       <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" t="s">
         <v>27</v>
       </c>
       <c r="O4" t="s">
@@ -1271,7 +1072,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1311,7 +1112,7 @@
       <c r="M5" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" t="s">
         <v>27</v>
       </c>
       <c r="O5" t="s">
@@ -1326,7 +1127,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1167,7 @@
       <c r="M6" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" t="s">
         <v>27</v>
       </c>
       <c r="O6" t="s">
@@ -1381,7 +1182,7 @@
         <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1421,7 +1222,7 @@
       <c r="M7" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" t="s">
         <v>27</v>
       </c>
       <c r="O7" t="s">
@@ -1436,7 +1237,7 @@
         <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1476,7 +1277,7 @@
       <c r="M8" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" t="s">
         <v>27</v>
       </c>
       <c r="O8" t="s">
@@ -1491,7 +1292,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1546,7 +1347,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1586,14 +1387,14 @@
       <c r="M10" t="s">
         <v>54</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" t="s">
         <v>55</v>
       </c>
       <c r="O10" t="s">
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P47" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P49" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1601,7 +1402,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1641,7 +1442,7 @@
       <c r="M11" t="s">
         <v>59</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" t="s">
         <v>55</v>
       </c>
       <c r="O11" t="s">
@@ -1652,11 +1453,11 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q47" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q49" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1696,7 +1497,7 @@
       <c r="M12" t="s">
         <v>64</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" t="s">
         <v>55</v>
       </c>
       <c r="O12" t="s">
@@ -1711,7 +1512,7 @@
         <v>mpox_outbreak_eue_2022_linelist_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1751,7 +1552,7 @@
       <c r="M13" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" t="s">
         <v>55</v>
       </c>
       <c r="O13" t="s">
@@ -1766,7 +1567,7 @@
         <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1806,7 +1607,7 @@
       <c r="M14" t="s">
         <v>72</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N14" t="s">
         <v>55</v>
       </c>
       <c r="O14" t="s">
@@ -1821,8 +1622,8 @@
         <v>salmonella_outbreak_deu_1998_linelist_1_1_outbreak_1998</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>73</v>
       </c>
       <c r="B15" t="s">
@@ -1876,7 +1677,7 @@
         <v>influenza_outbreak_chn_2013_linelist_1_1_outbreak_2013</v>
       </c>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1913,7 +1714,7 @@
       <c r="L16">
         <v>2014</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" t="s">
         <v>83</v>
       </c>
       <c r="N16" t="s">
@@ -1931,7 +1732,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1968,7 +1769,7 @@
       <c r="L17">
         <v>2014</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" t="s">
         <v>85</v>
       </c>
       <c r="N17" t="s">
@@ -1986,7 +1787,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_2_outbreak_2014</v>
       </c>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -2041,7 +1842,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_3_outbreak_2014</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2096,7 +1897,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_4_outbreak_2014</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -2133,7 +1934,7 @@
       <c r="L20">
         <v>2014</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" t="s">
         <v>91</v>
       </c>
       <c r="N20" t="s">
@@ -2151,7 +1952,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_5_outbreak_2014</v>
       </c>
     </row>
-    <row r="21" ht="14.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2206,7 +2007,7 @@
         <v>ebola_outbreak_sle_2014_dictionary_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="22" ht="14.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2261,7 +2062,7 @@
         <v>ebola_outbreak_sle_2014_shape_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -2304,7 +2105,7 @@
       <c r="N23" t="s">
         <v>78</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" t="s">
         <v>96</v>
       </c>
       <c r="P23" t="str">
@@ -2316,8 +2117,8 @@
         <v>ebola_outbreak_sle_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="24" ht="15.75">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B24" t="s">
@@ -2359,7 +2160,7 @@
       <c r="N24" t="s">
         <v>78</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" t="s">
         <v>79</v>
       </c>
       <c r="P24" t="str">
@@ -2371,8 +2172,8 @@
         <v>ebola_outbreak_sle_2014_other_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="25" ht="15.75">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B25" t="s">
@@ -2426,14 +2227,14 @@
         <v>ebola_outbreak_sle_2014_other_2_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="26" ht="14.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>57</v>
       </c>
       <c r="D26">
@@ -2442,22 +2243,22 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" t="s">
         <v>75</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" t="s">
         <v>82</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" t="s">
         <v>24</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" t="s">
         <v>42</v>
       </c>
       <c r="L26">
@@ -2481,7 +2282,7 @@
         <v>ebola_outbreak_sle_2014_other_3_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="27" ht="14.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2518,13 +2319,13 @@
       <c r="L27">
         <v>2014</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="N27" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="O27" t="s">
         <v>79</v>
       </c>
       <c r="P27" t="str">
@@ -2536,7 +2337,7 @@
         <v>ebola_outbreak_sle_2014_other_4_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="28" ht="14.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2591,14 +2392,14 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="29" ht="14.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>57</v>
       </c>
       <c r="D29">
@@ -2607,34 +2408,34 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
         <v>40</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="K29" t="s">
         <v>42</v>
       </c>
       <c r="L29">
         <v>2020</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="M29" t="s">
         <v>108</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="N29" t="s">
         <v>78</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="O29" t="s">
         <v>44</v>
       </c>
       <c r="P29" t="str">
@@ -2646,14 +2447,14 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_2_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="30" ht="14.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>57</v>
       </c>
       <c r="D30">
@@ -2662,34 +2463,34 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" t="s">
         <v>24</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" t="s">
         <v>42</v>
       </c>
       <c r="L30">
         <v>2020</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="M30" t="s">
         <v>108</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="N30" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="O30" t="s">
         <v>44</v>
       </c>
       <c r="P30" t="str">
@@ -2701,14 +2502,14 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_3_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="31" ht="14.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>57</v>
       </c>
       <c r="D31">
@@ -2717,34 +2518,34 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" t="s">
         <v>107</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J31" t="s">
         <v>24</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="K31" t="s">
         <v>42</v>
       </c>
       <c r="L31">
         <v>2020</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="M31" t="s">
         <v>108</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="N31" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="O31" t="s">
         <v>44</v>
       </c>
       <c r="P31" t="str">
@@ -2756,11 +2557,11 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_4_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="32" ht="14.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s">
         <v>66</v>
       </c>
       <c r="C32" t="s">
@@ -2799,7 +2600,7 @@
       <c r="N32" t="s">
         <v>78</v>
       </c>
-      <c r="O32" s="4" t="s">
+      <c r="O32" t="s">
         <v>28</v>
       </c>
       <c r="P32" t="str">
@@ -2811,7 +2612,7 @@
         <v>malaria_outbreak_moz_2019_aggregate_1_1_outbreak_2019</v>
       </c>
     </row>
-    <row r="33" ht="14.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2854,7 +2655,7 @@
       <c r="N33" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="4" t="s">
+      <c r="O33" t="s">
         <v>28</v>
       </c>
       <c r="P33" t="str">
@@ -2866,7 +2667,7 @@
         <v>malaria_outbreak_moz_2019_aggregate_1_2_outbreak_2019</v>
       </c>
     </row>
-    <row r="34" ht="14.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -2909,7 +2710,7 @@
       <c r="N34" t="s">
         <v>78</v>
       </c>
-      <c r="O34" s="4" t="s">
+      <c r="O34" t="s">
         <v>28</v>
       </c>
       <c r="P34" t="str">
@@ -2921,7 +2722,7 @@
         <v>shigella_surveillance_bel_2013_sequencing_1_1_surveillance_2013</v>
       </c>
     </row>
-    <row r="35" ht="15.5" customHeight="1">
+    <row r="35" spans="1:17" ht="15.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2958,13 +2759,13 @@
       <c r="L35">
         <v>2013</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M35" s="3" t="s">
         <v>125</v>
       </c>
       <c r="N35" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="4" t="s">
+      <c r="O35" t="s">
         <v>28</v>
       </c>
       <c r="P35" t="str">
@@ -2976,7 +2777,7 @@
         <v>shigella_surveillance_bel_2013_linelist_1_1_surveillance_2013</v>
       </c>
     </row>
-    <row r="36" ht="14.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -3013,13 +2814,13 @@
       <c r="L36">
         <v>2013</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="M36" t="s">
         <v>127</v>
       </c>
       <c r="N36" t="s">
         <v>78</v>
       </c>
-      <c r="O36" s="4" t="s">
+      <c r="O36" t="s">
         <v>28</v>
       </c>
       <c r="P36" t="str">
@@ -3031,7 +2832,7 @@
         <v>shigella_surveillance_bel_2013_sequencing_1_2_surveillance_2013</v>
       </c>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -3074,7 +2875,7 @@
       <c r="N37" t="s">
         <v>78</v>
       </c>
-      <c r="O37" s="4" t="s">
+      <c r="O37" t="s">
         <v>28</v>
       </c>
       <c r="P37" t="str">
@@ -3086,7 +2887,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_1_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3102,34 +2903,34 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
         <v>40</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" t="s">
         <v>75</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" t="s">
         <v>41</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" t="s">
         <v>122</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" t="s">
         <v>42</v>
       </c>
       <c r="L38">
         <v>2020</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" t="s">
         <v>129</v>
       </c>
       <c r="N38" t="s">
         <v>78</v>
       </c>
-      <c r="O38" s="4" t="s">
+      <c r="O38" t="s">
         <v>28</v>
       </c>
       <c r="P38" t="str">
@@ -3141,7 +2942,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_2_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -3157,34 +2958,34 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" t="s">
         <v>40</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" t="s">
         <v>75</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" t="s">
         <v>41</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" t="s">
         <v>122</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" t="s">
         <v>42</v>
       </c>
       <c r="L39">
         <v>2020</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" t="s">
         <v>129</v>
       </c>
       <c r="N39" t="s">
         <v>78</v>
       </c>
-      <c r="O39" s="4" t="s">
+      <c r="O39" t="s">
         <v>28</v>
       </c>
       <c r="P39" t="str">
@@ -3196,8 +2997,8 @@
         <v>mortality_surveillance_zzz_2020_aggregate_3_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="40" ht="14.25">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>132</v>
       </c>
       <c r="B40" t="s">
@@ -3212,34 +3013,34 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="2" t="s">
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" t="s">
         <v>40</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" t="s">
         <v>75</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" t="s">
         <v>41</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="J40" t="s">
         <v>122</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K40" t="s">
         <v>42</v>
       </c>
       <c r="L40">
         <v>2020</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="M40" t="s">
         <v>129</v>
       </c>
       <c r="N40" t="s">
         <v>78</v>
       </c>
-      <c r="O40" s="4" t="s">
+      <c r="O40" t="s">
         <v>28</v>
       </c>
       <c r="P40" t="str">
@@ -3251,7 +3052,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_4_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="41" ht="14.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3267,25 +3068,25 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="s">
         <v>40</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" t="s">
         <v>75</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" t="s">
         <v>41</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" t="s">
         <v>122</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="K41" t="s">
         <v>42</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41">
         <v>2020</v>
       </c>
       <c r="M41" t="s">
@@ -3294,7 +3095,7 @@
       <c r="N41" t="s">
         <v>78</v>
       </c>
-      <c r="O41" s="4" t="s">
+      <c r="O41" t="s">
         <v>135</v>
       </c>
       <c r="P41" t="str">
@@ -3306,7 +3107,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_5_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="42" ht="14.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -3361,7 +3162,7 @@
         <v>likert_other_zzz_2020_aggregate_1_1_other_2020</v>
       </c>
     </row>
-    <row r="43" ht="14.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3398,13 +3199,13 @@
       <c r="L43">
         <v>2021</v>
       </c>
-      <c r="M43" s="4" t="s">
+      <c r="M43" t="s">
         <v>140</v>
       </c>
       <c r="N43" t="s">
         <v>78</v>
       </c>
-      <c r="O43" s="4" t="s">
+      <c r="O43" t="s">
         <v>44</v>
       </c>
       <c r="P43" t="str">
@@ -3416,7 +3217,7 @@
         <v>mortality_survey_zzz_2021_survey_2_1_survey_2021</v>
       </c>
     </row>
-    <row r="44" ht="14.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3453,7 +3254,7 @@
       <c r="L44">
         <v>2021</v>
       </c>
-      <c r="M44" s="4" t="s">
+      <c r="M44" t="s">
         <v>142</v>
       </c>
       <c r="N44" t="s">
@@ -3471,7 +3272,7 @@
         <v>mortality_survey_zzz_2021_dictionary_2_1_survey_2021</v>
       </c>
     </row>
-    <row r="45" ht="14.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -3508,7 +3309,7 @@
       <c r="L45">
         <v>2021</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="M45" t="s">
         <v>143</v>
       </c>
       <c r="N45" t="s">
@@ -3526,7 +3327,7 @@
         <v>mortality_survey_zzz_2021_population_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="46" ht="14.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>144</v>
       </c>
@@ -3581,7 +3382,7 @@
         <v>campylobacter_surveillance_deu_2001_linelist_1_1_surveillance_2001</v>
       </c>
     </row>
-    <row r="47" ht="14.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>147</v>
       </c>
@@ -3636,62 +3437,129 @@
         <v>weather_other_deu_2001_aggregate_1_1_other_2001</v>
       </c>
     </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H48" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L48">
+        <v>2024</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N48" t="s">
+        <v>55</v>
+      </c>
+      <c r="O48" t="s">
+        <v>28</v>
+      </c>
+      <c r="P48" t="str">
+        <f>_xlfn.CONCAT(SUBSTITUTE(I48," ",""),"_",J48,"_",G48,"_",L48)</f>
+        <v>multidisease_tests_zzz_2024</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="3"/>
+        <v>multidisease_tests_zzz_2024_linelist_1_1_tests_2024</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H49" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L49">
+        <v>2024</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N49" t="s">
+        <v>55</v>
+      </c>
+      <c r="O49" t="s">
+        <v>28</v>
+      </c>
+      <c r="P49" t="str">
+        <f t="shared" si="2"/>
+        <v>multidisease_notifications_zzz_2024</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" si="3"/>
+        <v>multidisease_notifications_zzz_2024_linelist_1_1_notifications_2024</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{0055004F-0014-45DA-83AE-00F000D100EE}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A:A</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{009200FD-0052-46AC-BD0D-005200B000CF}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00AE00D8-0093-4F3E-B507-0037005F00C1}">
-            <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor indexed="2"/>
-                  <bgColor indexed="2"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G2:G25 G27:G28 G32:G37 G42:G300 G26 G29 G30 G31 G38 G39 G40 G41</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G300">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added datasets for multidisease case study
Added French, Spanish and Portuguese datasets (6) for the multidisease case study. Followed all instructions.
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanahjansen/Documents/GitHub/appliedepidata/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E197E55-7909-4234-9C93-6489C7F5E6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D7A75B-EDC9-DA45-AEB4-784D51512EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36920" yWindow="520" windowWidth="34520" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="163">
   <si>
     <t>name</t>
   </si>
@@ -498,6 +498,30 @@
   </si>
   <si>
     <t>multidisease</t>
+  </si>
+  <si>
+    <t>multi_maladies_notifications</t>
+  </si>
+  <si>
+    <t>multi_maladies_tests</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>pruebas_multienfermedad</t>
+  </si>
+  <si>
+    <t>notificaciones_multienfermedad</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>testes_multidoencas</t>
+  </si>
+  <si>
+    <t>notificacoes_multidoencas</t>
   </si>
 </sst>
 </file>
@@ -833,30 +857,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="Y43" sqref="Y43"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.68359375" bestFit="1"/>
-    <col min="2" max="2" width="10.26171875" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="9"/>
-    <col min="4" max="5" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.68359375" bestFit="1"/>
-    <col min="9" max="9" width="22.578125" bestFit="1"/>
-    <col min="10" max="11" width="11.15625" customWidth="1"/>
-    <col min="12" max="12" width="5.68359375" customWidth="1"/>
-    <col min="13" max="13" width="10.578125" bestFit="1"/>
-    <col min="14" max="14" width="18.15625" bestFit="1"/>
-    <col min="15" max="15" width="14.3125" bestFit="1"/>
-    <col min="16" max="16" width="39.68359375" bestFit="1"/>
-    <col min="17" max="17" width="67.41796875" bestFit="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1"/>
+    <col min="10" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1"/>
+    <col min="16" max="16" width="39.6640625" bestFit="1"/>
+    <col min="17" max="17" width="67.5" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -964,7 +988,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1019,7 +1043,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1098,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1129,7 +1153,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1184,7 +1208,7 @@
         <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1239,7 +1263,7 @@
         <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1294,7 +1318,7 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1349,7 +1373,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1396,7 +1420,7 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P49" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P51" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
@@ -1404,7 +1428,7 @@
         <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1455,11 +1479,11 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q49" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
+        <f t="shared" ref="Q11:Q51" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1514,7 +1538,7 @@
         <v>mpox_outbreak_eue_2022_linelist_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1569,7 +1593,7 @@
         <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1624,7 +1648,7 @@
         <v>salmonella_outbreak_deu_1998_linelist_1_1_outbreak_1998</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>influenza_outbreak_chn_2013_linelist_1_1_outbreak_2013</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1734,7 +1758,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1789,7 +1813,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_2_outbreak_2014</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1844,7 +1868,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_3_outbreak_2014</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1899,7 +1923,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_4_outbreak_2014</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1954,7 +1978,7 @@
         <v>ebola_outbreak_sle_2014_linelist_1_5_outbreak_2014</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2009,7 +2033,7 @@
         <v>ebola_outbreak_sle_2014_dictionary_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2064,7 +2088,7 @@
         <v>ebola_outbreak_sle_2014_shape_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -2119,7 +2143,7 @@
         <v>ebola_outbreak_sle_2020_population_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
@@ -2174,7 +2198,7 @@
         <v>ebola_outbreak_sle_2014_other_1_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
@@ -2229,7 +2253,7 @@
         <v>ebola_outbreak_sle_2014_other_2_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -2284,7 +2308,7 @@
         <v>ebola_outbreak_sle_2014_other_3_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2339,7 +2363,7 @@
         <v>ebola_outbreak_sle_2014_other_4_1_outbreak_2014</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2394,7 +2418,7 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_1_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -2449,7 +2473,7 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_2_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2504,7 +2528,7 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_3_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2559,7 +2583,7 @@
         <v>contacttracing_outbreak_zzz_2020_linelist_4_1_outbreak_2020</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2614,7 +2638,7 @@
         <v>malaria_outbreak_moz_2019_aggregate_1_1_outbreak_2019</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2669,7 +2693,7 @@
         <v>malaria_outbreak_moz_2019_aggregate_1_2_outbreak_2019</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -2724,7 +2748,7 @@
         <v>shigella_surveillance_bel_2013_sequencing_1_1_surveillance_2013</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2779,7 +2803,7 @@
         <v>shigella_surveillance_bel_2013_linelist_1_1_surveillance_2013</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -2834,7 +2858,7 @@
         <v>shigella_surveillance_bel_2013_sequencing_1_2_surveillance_2013</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -2889,7 +2913,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_1_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -2944,7 +2968,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_2_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -2999,7 +3023,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_3_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -3054,7 +3078,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_4_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3109,7 +3133,7 @@
         <v>mortality_surveillance_zzz_2020_aggregate_5_1_surveillance_2020</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -3164,7 +3188,7 @@
         <v>likert_other_zzz_2020_aggregate_1_1_other_2020</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3219,7 +3243,7 @@
         <v>mortality_survey_zzz_2021_survey_2_1_survey_2021</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3274,7 +3298,7 @@
         <v>mortality_survey_zzz_2021_dictionary_2_1_survey_2021</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -3329,7 +3353,7 @@
         <v>mortality_survey_zzz_2021_population_1_1_survey_2021</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>144</v>
       </c>
@@ -3384,7 +3408,7 @@
         <v>campylobacter_surveillance_deu_2001_linelist_1_1_surveillance_2001</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>147</v>
       </c>
@@ -3439,7 +3463,7 @@
         <v>weather_other_deu_2001_aggregate_1_1_other_2001</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>152</v>
       </c>
@@ -3494,7 +3518,7 @@
         <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>153</v>
       </c>
@@ -3549,8 +3573,338 @@
         <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
       </c>
     </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" t="s">
+        <v>75</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J50" t="s">
+        <v>122</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L50">
+        <v>2024</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N50" t="s">
+        <v>55</v>
+      </c>
+      <c r="O50" t="s">
+        <v>28</v>
+      </c>
+      <c r="P50" t="str">
+        <f t="shared" si="2"/>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" si="3"/>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J51" t="s">
+        <v>122</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L51">
+        <v>2024</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N51" t="s">
+        <v>55</v>
+      </c>
+      <c r="O51" t="s">
+        <v>28</v>
+      </c>
+      <c r="P51" t="str">
+        <f t="shared" si="2"/>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="3"/>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J52" t="s">
+        <v>122</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L52">
+        <v>2024</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N52" t="s">
+        <v>55</v>
+      </c>
+      <c r="O52" t="s">
+        <v>28</v>
+      </c>
+      <c r="P52" t="str">
+        <f t="shared" ref="P52:P53" si="4">_xlfn.CONCAT(SUBSTITUTE(I52," ",""),"_",J52,"_",G52,"_",L52)</f>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" ref="Q52:Q53" si="5">_xlfn.CONCAT(P52,"_",B52,"_",D52,"_",E52,"_",J52,"_",L52)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" t="s">
+        <v>75</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J53" t="s">
+        <v>122</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L53">
+        <v>2024</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N53" t="s">
+        <v>55</v>
+      </c>
+      <c r="O53" t="s">
+        <v>28</v>
+      </c>
+      <c r="P53" t="str">
+        <f t="shared" si="4"/>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="5"/>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J54" t="s">
+        <v>122</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L54">
+        <v>2024</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N54" t="s">
+        <v>55</v>
+      </c>
+      <c r="O54" t="s">
+        <v>28</v>
+      </c>
+      <c r="P54" t="str">
+        <f t="shared" ref="P54:P55" si="6">_xlfn.CONCAT(SUBSTITUTE(I54," ",""),"_",J54,"_",G54,"_",L54)</f>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" ref="Q54:Q55" si="7">_xlfn.CONCAT(P54,"_",B54,"_",D54,"_",E54,"_",J54,"_",L54)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="J55" t="s">
+        <v>122</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L55">
+        <v>2024</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N55" t="s">
+        <v>55</v>
+      </c>
+      <c r="O55" t="s">
+        <v>28</v>
+      </c>
+      <c r="P55" t="str">
+        <f t="shared" si="6"/>
+        <v>multidisease_surveillance_zzz_2024</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="7"/>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A1:A53 A56:A1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
update tableoftables for Redundant unique identifier in tableoftables Fixes #27
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,39 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanahjansen/Documents/GitHub/appliedepidata/inst/extdata/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D7A75B-EDC9-DA45-AEB4-784D51512EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36920" yWindow="520" windowWidth="34520" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>name</t>
   </si>
@@ -104,7 +87,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t>acute jaundice syndrome</t>
+    <t xml:space="preserve">acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -113,13 +96,13 @@
     <t>no</t>
   </si>
   <si>
-    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
   </si>
   <si>
     <t>sitrep_walkthroughs</t>
   </si>
   <si>
-    <t>CC by-NC-SA 4.0</t>
+    <t xml:space="preserve">CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -128,7 +111,7 @@
     <t>population</t>
   </si>
   <si>
-    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -140,13 +123,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -164,7 +147,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Fake data for a mortality survey</t>
+    <t xml:space="preserve">Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -176,7 +159,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t>Fake data dictionary for a mortality survey</t>
+    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -185,7 +168,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t>quelque chose en francais - oui oui</t>
+    <t xml:space="preserve">quelque chose en francais - oui oui</t>
   </si>
   <si>
     <t>fulton_data</t>
@@ -197,7 +180,7 @@
     <t>covid-19</t>
   </si>
   <si>
-    <t>Jittered COVID-19 linelist data from Fulton County</t>
+    <t xml:space="preserve">Jittered COVID-19 linelist data from Fulton County</t>
   </si>
   <si>
     <t>case_studies</t>
@@ -227,7 +210,7 @@
     <t>mpox</t>
   </si>
   <si>
-    <t>Fictional mpox case linelist in five European countries</t>
+    <t xml:space="preserve">Fictional mpox case linelist in five European countries</t>
   </si>
   <si>
     <t>mpox_aggregate_table</t>
@@ -239,7 +222,7 @@
     <t>csv</t>
   </si>
   <si>
-    <t>Fictional cumulative mpox case counts in five European countries</t>
+    <t xml:space="preserve">Fictional cumulative mpox case counts in five European countries</t>
   </si>
   <si>
     <t>stegentira_data</t>
@@ -251,7 +234,7 @@
     <t>salmonella</t>
   </si>
   <si>
-    <t>Fictional linelist of salmonella outbreak in Stegen, Germany</t>
+    <t xml:space="preserve">Fictional linelist of salmonella outbreak in Stegen, Germany</t>
   </si>
   <si>
     <t>fluH7N9_China_2013</t>
@@ -266,7 +249,7 @@
     <t>influenza</t>
   </si>
   <si>
-    <t>Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
+    <t xml:space="preserve">Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
   </si>
   <si>
     <t>epirhandbook</t>
@@ -284,52 +267,52 @@
     <t>ebola</t>
   </si>
   <si>
-    <t>Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_excel</t>
   </si>
   <si>
-    <t>Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_rds</t>
   </si>
   <si>
-    <t>R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>hospital_linelists</t>
   </si>
   <si>
-    <t>Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_with_adm3</t>
   </si>
   <si>
-    <t>Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>cleaning_dict</t>
   </si>
   <si>
-    <t>Short example cleaning dictionary for the raw linelist</t>
+    <t xml:space="preserve">Short example cleaning dictionary for the raw linelist</t>
   </si>
   <si>
     <t>sle_adm3</t>
   </si>
   <si>
-    <t>Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
-  </si>
-  <si>
-    <t>CC by-IGO</t>
+    <t xml:space="preserve">Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC by-IGO</t>
   </si>
   <si>
     <t>sle_admpop_adm3_2020</t>
   </si>
   <si>
-    <t>Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
+    <t xml:space="preserve">Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
   </si>
   <si>
     <t>epinow_res</t>
@@ -338,7 +321,7 @@
     <t>other</t>
   </si>
   <si>
-    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>epinow_res_small</t>
@@ -347,7 +330,7 @@
     <t>generation_time</t>
   </si>
   <si>
-    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
+    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
   </si>
   <si>
     <t>incubation_period</t>
@@ -356,10 +339,10 @@
     <t>cases_clean</t>
   </si>
   <si>
-    <t>contact tracing</t>
-  </si>
-  <si>
-    <t>Fictional case data for a generic disease to demonstrate contact tracing</t>
+    <t xml:space="preserve">contact tracing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictional case data for a generic disease to demonstrate contact tracing</t>
   </si>
   <si>
     <t>contacts_clean</t>
@@ -380,7 +363,7 @@
     <t>malaria</t>
   </si>
   <si>
-    <t>Fictional counts of malaria cases from Mozambique</t>
+    <t xml:space="preserve">Fictional counts of malaria cases from Mozambique</t>
   </si>
   <si>
     <t>malaria_facility_count_data</t>
@@ -404,25 +387,25 @@
     <t>surveillance</t>
   </si>
   <si>
-    <t>Next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t xml:space="preserve">Next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>sample_data_Shigella_tree</t>
   </si>
   <si>
-    <t>Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
+    <t xml:space="preserve">Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
   </si>
   <si>
     <t>Shigella_subtree_2</t>
   </si>
   <si>
-    <t>Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t xml:space="preserve">Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>country_demographics</t>
   </si>
   <si>
-    <t>Fictional country demographic and mortality data to demonstrate standardisation</t>
+    <t xml:space="preserve">Fictional country demographic and mortality data to demonstrate standardisation</t>
   </si>
   <si>
     <t>country_demographics_2</t>
@@ -437,7 +420,7 @@
     <t>world_standard_population_by_sex</t>
   </si>
   <si>
-    <t>World “standard population” by sex</t>
+    <t xml:space="preserve">World “standard population” by sex</t>
   </si>
   <si>
     <t>OGL</t>
@@ -449,22 +432,22 @@
     <t>likert</t>
   </si>
   <si>
-    <t>Fictional likert data for demonstration purposes</t>
+    <t xml:space="preserve">Fictional likert data for demonstration purposes</t>
   </si>
   <si>
     <t>survey_data</t>
   </si>
   <si>
-    <t>Fictional data for a mortality survey</t>
+    <t xml:space="preserve">Fictional data for a mortality survey</t>
   </si>
   <si>
     <t>survey_dict</t>
   </si>
   <si>
-    <t>Fictional data dictionary for a mortality survey</t>
-  </si>
-  <si>
-    <t>Fictional population data for a mortality survey</t>
+    <t xml:space="preserve">Fictional data dictionary for a mortality survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictional population data for a mortality survey</t>
   </si>
   <si>
     <t>campylobacter_germany</t>
@@ -473,7 +456,7 @@
     <t>campylobacter</t>
   </si>
   <si>
-    <t>Campylobacter surveillance data from Germany</t>
+    <t xml:space="preserve">Campylobacter surveillance data from Germany</t>
   </si>
   <si>
     <t>germany_weather</t>
@@ -482,22 +465,22 @@
     <t>weather</t>
   </si>
   <si>
-    <t>Weather data for Germany from 2001-2011</t>
-  </si>
-  <si>
-    <t>Test results for notifiable diseases reported in Feveria in 2024</t>
-  </si>
-  <si>
-    <t>Notifiable disease surveillance data in Feveria in 2024</t>
+    <t xml:space="preserve">Weather data for Germany from 2001-2011</t>
   </si>
   <si>
     <t>multidisease_tests</t>
   </si>
   <si>
+    <t>multidisease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test results for notifiable diseases reported in Feveria in 2024</t>
+  </si>
+  <si>
     <t>multidisease_notifications</t>
   </si>
   <si>
-    <t>multidisease</t>
+    <t xml:space="preserve">Notifiable disease surveillance data in Feveria in 2024</t>
   </si>
   <si>
     <t>multi_maladies_notifications</t>
@@ -506,66 +489,49 @@
     <t>multi_maladies_tests</t>
   </si>
   <si>
+    <t>notificaciones_multienfermedad</t>
+  </si>
+  <si>
     <t>es</t>
   </si>
   <si>
     <t>pruebas_multienfermedad</t>
   </si>
   <si>
-    <t>notificaciones_multienfermedad</t>
+    <t>notificacoes_multidoencas</t>
   </si>
   <si>
     <t>pt</t>
   </si>
   <si>
     <t>testes_multidoencas</t>
-  </si>
-  <si>
-    <t>notificacoes_multidoencas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11.500000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -578,63 +544,31 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="2"/>
-          <bgColor indexed="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -647,8 +581,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -851,36 +1068,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="O1" zoomScale="100" workbookViewId="0">
+      <selection activeCell="M34" activeCellId="0" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col bestFit="1" min="1" max="1" width="24.6640625"/>
+    <col customWidth="1" min="2" max="2" width="10.33203125"/>
     <col min="3" max="3" width="9"/>
-    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1"/>
-    <col min="9" max="9" width="22.5" bestFit="1"/>
-    <col min="10" max="11" width="11.1640625" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1"/>
-    <col min="14" max="14" width="18.1640625" bestFit="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1"/>
-    <col min="16" max="16" width="39.6640625" bestFit="1"/>
-    <col min="17" max="17" width="67.5" bestFit="1"/>
+    <col bestFit="1" customWidth="1" min="4" max="5" width="12.1640625"/>
+    <col bestFit="1" min="8" max="8" width="10.6640625"/>
+    <col bestFit="1" min="9" max="9" width="22.5"/>
+    <col customWidth="1" min="10" max="11" width="11.1640625"/>
+    <col customWidth="1" min="12" max="12" width="5.6640625"/>
+    <col bestFit="1" min="13" max="13" width="10.5"/>
+    <col bestFit="1" min="14" max="14" width="18.1640625"/>
+    <col bestFit="1" min="15" max="15" width="14.33203125"/>
+    <col bestFit="1" min="16" max="16" width="39.6640625"/>
+    <col bestFit="1" min="17" max="17" width="67.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +1148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -984,11 +1199,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q10" si="1">_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2,"_",J2,"_",L2)</f>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2)</f>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1039,11 +1254,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1_outbreak_2016</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P3,"_",B3,"_",D3,"_",E3)</f>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1094,11 +1309,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1_outbreak_2016</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P4,"_",B4,"_",D4,"_",E4)</f>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1149,11 +1364,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1_outbreak_2016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P5,"_",B5,"_",D5,"_",E5)</f>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1204,11 +1419,11 @@
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="1"/>
-        <v>mortality_survey_zzz_2021_survey_1_1_survey_2021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P6,"_",B6,"_",D6,"_",E6)</f>
+        <v>mortality_survey_zzz_2021_survey_1_1</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1259,11 +1474,11 @@
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="1"/>
-        <v>mortality_survey_zzz_2021_dictionary_1_1_survey_2021</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P7,"_",B7,"_",D7,"_",E7)</f>
+        <v>mortality_survey_zzz_2021_dictionary_1_1</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1314,11 +1529,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="1"/>
-        <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1_outbreak_2016</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P8,"_",B8,"_",D8,"_",E8)</f>
+        <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1369,11 +1584,11 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="1"/>
-        <v>covid-19_outbreak_usa_2020_linelist_1_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P9,"_",B9,"_",D9,"_",E9)</f>
+        <v>covid-19_outbreak_usa_2020_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1420,15 +1635,15 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P51" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P55" si="1">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="1"/>
-        <v>covid-19_outbreak_usa_2020_linelist_1_2_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P10,"_",B10,"_",D10,"_",E10)</f>
+        <v>covid-19_outbreak_usa_2020_linelist_1_2</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1475,15 +1690,15 @@
         <v>28</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:Q51" si="3">_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11,"_",J11,"_",L11)</f>
-        <v>covid-19_outbreak_usa_2020_population_1_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11)</f>
+        <v>covid-19_outbreak_usa_2020_population_1_1</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1530,15 +1745,15 @@
         <v>28</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mpox_outbreak_eue_2022</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="3"/>
-        <v>mpox_outbreak_eue_2022_linelist_1_1_outbreak_2022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P12,"_",B12,"_",D12,"_",E12)</f>
+        <v>mpox_outbreak_eue_2022_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1585,15 +1800,15 @@
         <v>28</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mpox_outbreak_eue_2022</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="3"/>
-        <v>mpox_outbreak_eue_2022_aggregate_1_1_outbreak_2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P13,"_",B13,"_",D13,"_",E13)</f>
+        <v>mpox_outbreak_eue_2022_aggregate_1_1</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1640,15 +1855,15 @@
         <v>28</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>salmonella_outbreak_deu_1998</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="3"/>
-        <v>salmonella_outbreak_deu_1998_linelist_1_1_outbreak_1998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P14,"_",B14,"_",D14,"_",E14)</f>
+        <v>salmonella_outbreak_deu_1998_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1695,15 +1910,15 @@
         <v>79</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>influenza_outbreak_chn_2013</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="3"/>
-        <v>influenza_outbreak_chn_2013_linelist_1_1_outbreak_2013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P15,"_",B15,"_",D15,"_",E15)</f>
+        <v>influenza_outbreak_chn_2013_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1750,15 +1965,15 @@
         <v>79</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_linelist_1_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P16,"_",B16,"_",D16,"_",E16)</f>
+        <v>ebola_outbreak_sle_2014_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -1805,15 +2020,15 @@
         <v>79</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_linelist_1_2_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P17,"_",B17,"_",D17,"_",E17)</f>
+        <v>ebola_outbreak_sle_2014_linelist_1_2</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1860,15 +2075,15 @@
         <v>79</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_linelist_1_3_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P18,"_",B18,"_",D18,"_",E18)</f>
+        <v>ebola_outbreak_sle_2014_linelist_1_3</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1915,15 +2130,15 @@
         <v>79</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_linelist_1_4_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P19,"_",B19,"_",D19,"_",E19)</f>
+        <v>ebola_outbreak_sle_2014_linelist_1_4</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1970,15 +2185,15 @@
         <v>79</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_linelist_1_5_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P20,"_",B20,"_",D20,"_",E20)</f>
+        <v>ebola_outbreak_sle_2014_linelist_1_5</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2025,15 +2240,15 @@
         <v>79</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_dictionary_1_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P21,"_",B21,"_",D21,"_",E21)</f>
+        <v>ebola_outbreak_sle_2014_dictionary_1_1</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2080,15 +2295,15 @@
         <v>96</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_shape_1_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P22,"_",B22,"_",D22,"_",E22)</f>
+        <v>ebola_outbreak_sle_2014_shape_1_1</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -2135,15 +2350,15 @@
         <v>96</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2020</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2020_population_1_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P23,"_",B23,"_",D23,"_",E23)</f>
+        <v>ebola_outbreak_sle_2020_population_1_1</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
@@ -2190,15 +2405,15 @@
         <v>79</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_other_1_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P24,"_",B24,"_",D24,"_",E24)</f>
+        <v>ebola_outbreak_sle_2014_other_1_1</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
@@ -2245,15 +2460,15 @@
         <v>79</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_other_2_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P25,"_",B25,"_",D25,"_",E25)</f>
+        <v>ebola_outbreak_sle_2014_other_2_1</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -2300,15 +2515,15 @@
         <v>79</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_other_3_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P26,"_",B26,"_",D26,"_",E26)</f>
+        <v>ebola_outbreak_sle_2014_other_3_1</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2355,15 +2570,15 @@
         <v>79</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ebola_outbreak_sle_2014</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="3"/>
-        <v>ebola_outbreak_sle_2014_other_4_1_outbreak_2014</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P27,"_",B27,"_",D27,"_",E27)</f>
+        <v>ebola_outbreak_sle_2014_other_4_1</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2410,15 +2625,15 @@
         <v>44</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="3"/>
-        <v>contacttracing_outbreak_zzz_2020_linelist_1_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P28,"_",B28,"_",D28,"_",E28)</f>
+        <v>contacttracing_outbreak_zzz_2020_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -2465,15 +2680,15 @@
         <v>44</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="3"/>
-        <v>contacttracing_outbreak_zzz_2020_linelist_2_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P29,"_",B29,"_",D29,"_",E29)</f>
+        <v>contacttracing_outbreak_zzz_2020_linelist_2_1</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2520,15 +2735,15 @@
         <v>44</v>
       </c>
       <c r="P30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="3"/>
-        <v>contacttracing_outbreak_zzz_2020_linelist_3_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P30,"_",B30,"_",D30,"_",E30)</f>
+        <v>contacttracing_outbreak_zzz_2020_linelist_3_1</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2575,15 +2790,15 @@
         <v>44</v>
       </c>
       <c r="P31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>contacttracing_outbreak_zzz_2020</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="3"/>
-        <v>contacttracing_outbreak_zzz_2020_linelist_4_1_outbreak_2020</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P31,"_",B31,"_",D31,"_",E31)</f>
+        <v>contacttracing_outbreak_zzz_2020_linelist_4_1</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2630,15 +2845,15 @@
         <v>28</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>malaria_outbreak_moz_2019</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="3"/>
-        <v>malaria_outbreak_moz_2019_aggregate_1_1_outbreak_2019</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P32,"_",B32,"_",D32,"_",E32)</f>
+        <v>malaria_outbreak_moz_2019_aggregate_1_1</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2685,15 +2900,15 @@
         <v>28</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>malaria_outbreak_moz_2019</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="3"/>
-        <v>malaria_outbreak_moz_2019_aggregate_1_2_outbreak_2019</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P33,"_",B33,"_",D33,"_",E33)</f>
+        <v>malaria_outbreak_moz_2019_aggregate_1_2</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -2740,15 +2955,15 @@
         <v>28</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="3"/>
-        <v>shigella_surveillance_bel_2013_sequencing_1_1_surveillance_2013</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P34,"_",B34,"_",D34,"_",E34)</f>
+        <v>shigella_surveillance_bel_2013_sequencing_1_1</v>
+      </c>
+    </row>
+    <row r="35" ht="15.5" customHeight="1">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2795,15 +3010,15 @@
         <v>28</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="3"/>
-        <v>shigella_surveillance_bel_2013_linelist_1_1_surveillance_2013</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P35,"_",B35,"_",D35,"_",E35)</f>
+        <v>shigella_surveillance_bel_2013_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -2850,15 +3065,15 @@
         <v>28</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="3"/>
-        <v>shigella_surveillance_bel_2013_sequencing_1_2_surveillance_2013</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P36,"_",B36,"_",D36,"_",E36)</f>
+        <v>shigella_surveillance_bel_2013_sequencing_1_2</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -2905,15 +3120,15 @@
         <v>28</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_surveillance_zzz_2020_aggregate_1_1_surveillance_2020</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P37,"_",B37,"_",D37,"_",E37)</f>
+        <v>mortality_surveillance_zzz_2020_aggregate_1_1</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -2960,15 +3175,15 @@
         <v>28</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_surveillance_zzz_2020_aggregate_2_1_surveillance_2020</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P38,"_",B38,"_",D38,"_",E38)</f>
+        <v>mortality_surveillance_zzz_2020_aggregate_2_1</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -3015,15 +3230,15 @@
         <v>28</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_surveillance_zzz_2020_aggregate_3_1_surveillance_2020</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P39,"_",B39,"_",D39,"_",E39)</f>
+        <v>mortality_surveillance_zzz_2020_aggregate_3_1</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -3070,15 +3285,15 @@
         <v>28</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_surveillance_zzz_2020_aggregate_4_1_surveillance_2020</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P40,"_",B40,"_",D40,"_",E40)</f>
+        <v>mortality_surveillance_zzz_2020_aggregate_4_1</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3125,15 +3340,15 @@
         <v>135</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_surveillance_zzz_2020_aggregate_5_1_surveillance_2020</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P41,"_",B41,"_",D41,"_",E41)</f>
+        <v>mortality_surveillance_zzz_2020_aggregate_5_1</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -3180,15 +3395,15 @@
         <v>28</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>likert_other_zzz_2020</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" si="3"/>
-        <v>likert_other_zzz_2020_aggregate_1_1_other_2020</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P42,"_",B42,"_",D42,"_",E42)</f>
+        <v>likert_other_zzz_2020_aggregate_1_1</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3235,15 +3450,15 @@
         <v>44</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_survey_zzz_2021_survey_2_1_survey_2021</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P43,"_",B43,"_",D43,"_",E43)</f>
+        <v>mortality_survey_zzz_2021_survey_2_1</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3290,15 +3505,15 @@
         <v>44</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_survey_zzz_2021_dictionary_2_1_survey_2021</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P44,"_",B44,"_",D44,"_",E44)</f>
+        <v>mortality_survey_zzz_2021_dictionary_2_1</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -3345,15 +3560,15 @@
         <v>44</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" si="3"/>
-        <v>mortality_survey_zzz_2021_population_1_1_survey_2021</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P45,"_",B45,"_",D45,"_",E45)</f>
+        <v>mortality_survey_zzz_2021_population_1_1</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" t="s">
         <v>144</v>
       </c>
@@ -3400,15 +3615,15 @@
         <v>44</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>campylobacter_surveillance_deu_2001</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" si="3"/>
-        <v>campylobacter_surveillance_deu_2001_linelist_1_1_surveillance_2001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P46,"_",B46,"_",D46,"_",E46)</f>
+        <v>campylobacter_surveillance_deu_2001_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" t="s">
         <v>147</v>
       </c>
@@ -3455,17 +3670,17 @@
         <v>44</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>weather_other_deu_2001</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" si="3"/>
-        <v>weather_other_deu_2001_aggregate_1_1_other_2001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P47,"_",B47,"_",D47,"_",E47)</f>
+        <v>weather_other_deu_2001_aggregate_1_1</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>18</v>
@@ -3488,8 +3703,8 @@
       <c r="H48" t="s">
         <v>75</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>154</v>
+      <c r="I48" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J48" t="s">
         <v>122</v>
@@ -3501,7 +3716,7 @@
         <v>2024</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N48" t="s">
         <v>55</v>
@@ -3510,15 +3725,15 @@
         <v>28</v>
       </c>
       <c r="P48" t="str">
-        <f>_xlfn.CONCAT(SUBSTITUTE(I48," ",""),"_",J48,"_",G48,"_",L48)</f>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" si="3"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P48,"_",B48,"_",D48,"_",E48)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49" s="4" t="s">
         <v>153</v>
       </c>
@@ -3544,7 +3759,7 @@
         <v>75</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J49" t="s">
         <v>122</v>
@@ -3556,7 +3771,7 @@
         <v>2024</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N49" t="s">
         <v>55</v>
@@ -3565,15 +3780,15 @@
         <v>28</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" si="3"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P49,"_",B49,"_",D49,"_",E49)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -3589,7 +3804,7 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>49</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -3599,7 +3814,7 @@
         <v>75</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J50" t="s">
         <v>122</v>
@@ -3611,7 +3826,7 @@
         <v>2024</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N50" t="s">
         <v>55</v>
@@ -3620,16 +3835,16 @@
         <v>28</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" si="3"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+        <f>_xlfn.CONCAT(P50,"_",B50,"_",D50,"_",E50)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -3644,7 +3859,7 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="4" t="s">
         <v>49</v>
       </c>
       <c r="G51" s="4" t="s">
@@ -3653,8 +3868,8 @@
       <c r="H51" t="s">
         <v>75</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>154</v>
+      <c r="I51" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J51" t="s">
         <v>122</v>
@@ -3666,7 +3881,7 @@
         <v>2024</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N51" t="s">
         <v>55</v>
@@ -3675,17 +3890,17 @@
         <v>28</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" si="3"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(P51,"_",B51,"_",D51,"_",E51)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>18</v>
@@ -3699,8 +3914,8 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>157</v>
+      <c r="F52" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>40</v>
@@ -3709,7 +3924,7 @@
         <v>75</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J52" t="s">
         <v>122</v>
@@ -3721,7 +3936,7 @@
         <v>2024</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N52" t="s">
         <v>55</v>
@@ -3730,17 +3945,17 @@
         <v>28</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" ref="P52:P53" si="4">_xlfn.CONCAT(SUBSTITUTE(I52," ",""),"_",J52,"_",G52,"_",L52)</f>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" ref="Q52:Q53" si="5">_xlfn.CONCAT(P52,"_",B52,"_",D52,"_",E52,"_",J52,"_",L52)</f>
-        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>158</v>
+        <f>_xlfn.CONCAT(P52,"_",B52,"_",D52,"_",E52)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>18</v>
@@ -3754,8 +3969,8 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>157</v>
+      <c r="F53" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>40</v>
@@ -3763,8 +3978,8 @@
       <c r="H53" t="s">
         <v>75</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>154</v>
+      <c r="I53" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J53" t="s">
         <v>122</v>
@@ -3776,7 +3991,7 @@
         <v>2024</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N53" t="s">
         <v>55</v>
@@ -3785,17 +4000,17 @@
         <v>28</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" si="5"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>162</v>
+        <f>_xlfn.CONCAT(P53,"_",B53,"_",D53,"_",E53)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>18</v>
@@ -3809,8 +4024,8 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>160</v>
+      <c r="F54" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>40</v>
@@ -3819,7 +4034,7 @@
         <v>75</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J54" t="s">
         <v>122</v>
@@ -3831,7 +4046,7 @@
         <v>2024</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N54" t="s">
         <v>55</v>
@@ -3840,17 +4055,17 @@
         <v>28</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" ref="P54:P55" si="6">_xlfn.CONCAT(SUBSTITUTE(I54," ",""),"_",J54,"_",G54,"_",L54)</f>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" ref="Q54:Q55" si="7">_xlfn.CONCAT(P54,"_",B54,"_",D54,"_",E54,"_",J54,"_",L54)</f>
-        <v>multidisease_surveillance_zzz_2024_linelist_2_1_surveillance_2024</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>161</v>
+        <f>_xlfn.CONCAT(P54,"_",B54,"_",D54,"_",E54)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>18</v>
@@ -3864,8 +4079,8 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="5" t="s">
-        <v>160</v>
+      <c r="F55" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>40</v>
@@ -3873,8 +4088,8 @@
       <c r="H55" t="s">
         <v>75</v>
       </c>
-      <c r="I55" s="5" t="s">
-        <v>154</v>
+      <c r="I55" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="J55" t="s">
         <v>122</v>
@@ -3886,7 +4101,7 @@
         <v>2024</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N55" t="s">
         <v>55</v>
@@ -3895,27 +4110,70 @@
         <v>28</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" si="7"/>
-        <v>multidisease_surveillance_zzz_2024_linelist_1_1_surveillance_2024</v>
+        <f>_xlfn.CONCAT(P55,"_",B55,"_",D55,"_",E55)</f>
+        <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A53 A56:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G300">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="duplicateValues" priority="3" id="{0074009D-0046-4C59-99FD-00C2004D0079}">
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A1:A53 A56:A1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="duplicateValues" priority="4" id="{00CB0073-008D-4E61-B735-005C00830098}">
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC7CE"/>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{00AF0095-00BF-4E5C-A5A2-004D00880094}">
+            <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor indexed="2"/>
+                  <bgColor indexed="2"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:G300</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data for qmd course/intro course - three releases of cholera data for Viraland
</commit_message>
<xml_diff>
--- a/inst/extdata/tableoftables.xlsx
+++ b/inst/extdata/tableoftables.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula Blomquist\Documents\R projects\appliedepidata\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9A25EE-4CE2-4881-8AAF-3432AD5A8F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-28920" yWindow="-3255" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="175">
   <si>
     <t>name</t>
   </si>
@@ -87,7 +104,7 @@
     <t>subnational</t>
   </si>
   <si>
-    <t xml:space="preserve">acute jaundice syndrome</t>
+    <t>acute jaundice syndrome</t>
   </si>
   <si>
     <t>outbreak</t>
@@ -96,13 +113,13 @@
     <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
+    <t>Linelist data from a real outbreak of Hepatitis E virus (HEV) infection which occurred in the town of Am Timan, Chad, between October 2016 and April 2017.</t>
   </si>
   <si>
     <t>sitrep_walkthroughs</t>
   </si>
   <si>
-    <t xml:space="preserve">CC by-NC-SA 4.0</t>
+    <t>CC by-NC-SA 4.0</t>
   </si>
   <si>
     <t>AJS_AmTiman_population</t>
@@ -111,7 +128,7 @@
     <t>population</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Population data from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Blocksshape</t>
@@ -123,13 +140,13 @@
     <t>zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of housing blocks from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>Quartiersshape</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
+    <t>Shapefile of neighbourhoods (fr: quartiers) from an outbreak of Acute Jaundice Syndrome (AJS) in Chad 2016</t>
   </si>
   <si>
     <t>mortality_survey_data</t>
@@ -147,7 +164,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data for a mortality survey</t>
+    <t>Fake data for a mortality survey</t>
   </si>
   <si>
     <t>gpl3</t>
@@ -159,7 +176,7 @@
     <t>dictionary</t>
   </si>
   <si>
-    <t xml:space="preserve">Fake data dictionary for a mortality survey</t>
+    <t>Fake data dictionary for a mortality survey</t>
   </si>
   <si>
     <t>franglais_AJS_AmTiman</t>
@@ -168,7 +185,7 @@
     <t>fr</t>
   </si>
   <si>
-    <t xml:space="preserve">quelque chose en francais - oui oui</t>
+    <t>quelque chose en francais - oui oui</t>
   </si>
   <si>
     <t>fulton_data</t>
@@ -180,7 +197,7 @@
     <t>covid-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Jittered COVID-19 linelist data from Fulton County</t>
+    <t>Jittered COVID-19 linelist data from Fulton County</t>
   </si>
   <si>
     <t>case_studies</t>
@@ -210,7 +227,7 @@
     <t>mpox</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional mpox case linelist in five European countries</t>
+    <t>Fictional mpox case linelist in five European countries</t>
   </si>
   <si>
     <t>mpox_aggregate_table</t>
@@ -222,7 +239,7 @@
     <t>csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional cumulative mpox case counts in five European countries</t>
+    <t>Fictional cumulative mpox case counts in five European countries</t>
   </si>
   <si>
     <t>stegentira_data</t>
@@ -234,7 +251,7 @@
     <t>salmonella</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional linelist of salmonella outbreak in Stegen, Germany</t>
+    <t>Fictional linelist of salmonella outbreak in Stegen, Germany</t>
   </si>
   <si>
     <t>fluH7N9_China_2013</t>
@@ -249,7 +266,7 @@
     <t>influenza</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
+    <t>Linelist data from an outbreak of influenza A H7N9 in China 2013.</t>
   </si>
   <si>
     <t>epirhandbook</t>
@@ -267,52 +284,52 @@
     <t>ebola</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_excel</t>
   </si>
   <si>
-    <t xml:space="preserve">Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_rds</t>
   </si>
   <si>
-    <t xml:space="preserve">R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>R-dataset clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>hospital_linelists</t>
   </si>
   <si>
-    <t xml:space="preserve">Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Subset of excel clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>linelist_cleaned_with_adm3</t>
   </si>
   <si>
-    <t xml:space="preserve">Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Subset with additional spatial data of rds clean version of fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>cleaning_dict</t>
   </si>
   <si>
-    <t xml:space="preserve">Short example cleaning dictionary for the raw linelist</t>
+    <t>Short example cleaning dictionary for the raw linelist</t>
   </si>
   <si>
     <t>sle_adm3</t>
   </si>
   <si>
-    <t xml:space="preserve">Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC by-IGO</t>
+    <t>Shapefile at admin level  3 for Sierra Leone from Humanitarian Data Exchange</t>
+  </si>
+  <si>
+    <t>CC by-IGO</t>
   </si>
   <si>
     <t>sle_admpop_adm3_2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
+    <t>Population data at admin level 3 for Sierra Leone from Humanitarian Data Exchange</t>
   </si>
   <si>
     <t>epinow_res</t>
@@ -321,7 +338,7 @@
     <t>other</t>
   </si>
   <si>
-    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
+    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2014</t>
   </si>
   <si>
     <t>epinow_res_small</t>
@@ -330,7 +347,7 @@
     <t>generation_time</t>
   </si>
   <si>
-    <t xml:space="preserve">Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
+    <t>Outputs from {epinow2} based on fictional Ebola Virus Disease data simulating properties from the West African Ebola outbreak of 2015</t>
   </si>
   <si>
     <t>incubation_period</t>
@@ -339,10 +356,10 @@
     <t>cases_clean</t>
   </si>
   <si>
-    <t xml:space="preserve">contact tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictional case data for a generic disease to demonstrate contact tracing</t>
+    <t>contact tracing</t>
+  </si>
+  <si>
+    <t>Fictional case data for a generic disease to demonstrate contact tracing</t>
   </si>
   <si>
     <t>contacts_clean</t>
@@ -363,7 +380,7 @@
     <t>malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional counts of malaria cases from Mozambique</t>
+    <t>Fictional counts of malaria cases from Mozambique</t>
   </si>
   <si>
     <t>malaria_facility_count_data</t>
@@ -387,25 +404,25 @@
     <t>surveillance</t>
   </si>
   <si>
-    <t xml:space="preserve">Next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t>Next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>sample_data_Shigella_tree</t>
   </si>
   <si>
-    <t xml:space="preserve">Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
+    <t>Linelist data to accompany next generation sequencing data of Shigella surveillance samples from Belgium 2013-2019</t>
   </si>
   <si>
     <t>Shigella_subtree_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
+    <t>Analysis output from next generation sequencing data of Shigella surveillance samples from Belgium</t>
   </si>
   <si>
     <t>country_demographics</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional country demographic and mortality data to demonstrate standardisation</t>
+    <t>Fictional country demographic and mortality data to demonstrate standardisation</t>
   </si>
   <si>
     <t>country_demographics_2</t>
@@ -420,7 +437,7 @@
     <t>world_standard_population_by_sex</t>
   </si>
   <si>
-    <t xml:space="preserve">World “standard population” by sex</t>
+    <t>World “standard population” by sex</t>
   </si>
   <si>
     <t>OGL</t>
@@ -432,22 +449,22 @@
     <t>likert</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional likert data for demonstration purposes</t>
+    <t>Fictional likert data for demonstration purposes</t>
   </si>
   <si>
     <t>survey_data</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional data for a mortality survey</t>
+    <t>Fictional data for a mortality survey</t>
   </si>
   <si>
     <t>survey_dict</t>
   </si>
   <si>
-    <t xml:space="preserve">Fictional data dictionary for a mortality survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictional population data for a mortality survey</t>
+    <t>Fictional data dictionary for a mortality survey</t>
+  </si>
+  <si>
+    <t>Fictional population data for a mortality survey</t>
   </si>
   <si>
     <t>campylobacter_germany</t>
@@ -456,7 +473,7 @@
     <t>campylobacter</t>
   </si>
   <si>
-    <t xml:space="preserve">Campylobacter surveillance data from Germany</t>
+    <t>Campylobacter surveillance data from Germany</t>
   </si>
   <si>
     <t>germany_weather</t>
@@ -465,7 +482,7 @@
     <t>weather</t>
   </si>
   <si>
-    <t xml:space="preserve">Weather data for Germany from 2001-2011</t>
+    <t>Weather data for Germany from 2001-2011</t>
   </si>
   <si>
     <t>multidisease_tests</t>
@@ -474,13 +491,13 @@
     <t>multidisease</t>
   </si>
   <si>
-    <t xml:space="preserve">Test results for notifiable diseases reported in Feveria in 2024</t>
+    <t>Test results for notifiable diseases reported in Feveria in 2024</t>
   </si>
   <si>
     <t>multidisease_notifications</t>
   </si>
   <si>
-    <t xml:space="preserve">Notifiable disease surveillance data in Feveria in 2024</t>
+    <t>Notifiable disease surveillance data in Feveria in 2024</t>
   </si>
   <si>
     <t>multi_maladies_notifications</t>
@@ -505,32 +522,68 @@
   </si>
   <si>
     <t>testes_multidoencas</t>
+  </si>
+  <si>
+    <t>cholera</t>
+  </si>
+  <si>
+    <t>Clean cholera surveillance data for Viraland, 17 June 2021</t>
+  </si>
+  <si>
+    <t>r_courses</t>
+  </si>
+  <si>
+    <t>Clean cholera surveillance data for Viraland, 25 May 2021</t>
+  </si>
+  <si>
+    <t>Clean cholera surveillance data for Viraland, 21 July 2021</t>
+  </si>
+  <si>
+    <t>Raw cholera surveillance data for Viraland, 21 July 2021</t>
+  </si>
+  <si>
+    <t>Raw cholera lab data for Viraland, 21 July 2021</t>
+  </si>
+  <si>
+    <t>viraland_cholera_20210721_labs</t>
+  </si>
+  <si>
+    <t>viraland_cholera_20210525_linelist</t>
+  </si>
+  <si>
+    <t>viraland_cholera_20210617_linelist</t>
+  </si>
+  <si>
+    <t>viraland_cholera_20210721_linelist</t>
+  </si>
+  <si>
+    <t>viraland_cholera_20210721_linelist_raw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.500000"/>
+      <sz val="11.5"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -544,31 +597,61 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="2"/>
+          <bgColor indexed="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -581,291 +664,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -1068,34 +868,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="100" workbookViewId="0">
-      <selection activeCell="M34" activeCellId="0" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="24.6640625"/>
-    <col customWidth="1" min="2" max="2" width="10.33203125"/>
+    <col min="1" max="1" width="44.26171875" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
     <col min="3" max="3" width="9"/>
-    <col bestFit="1" customWidth="1" min="4" max="5" width="12.1640625"/>
-    <col bestFit="1" min="8" max="8" width="10.6640625"/>
-    <col bestFit="1" min="9" max="9" width="22.5"/>
-    <col customWidth="1" min="10" max="11" width="11.1640625"/>
-    <col customWidth="1" min="12" max="12" width="5.6640625"/>
-    <col bestFit="1" min="13" max="13" width="10.5"/>
-    <col bestFit="1" min="14" max="14" width="18.1640625"/>
-    <col bestFit="1" min="15" max="15" width="14.33203125"/>
-    <col bestFit="1" min="16" max="16" width="39.6640625"/>
-    <col bestFit="1" min="17" max="17" width="67.5"/>
+    <col min="4" max="5" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.68359375" bestFit="1"/>
+    <col min="9" max="9" width="22.47265625" bestFit="1"/>
+    <col min="10" max="11" width="11.15625" customWidth="1"/>
+    <col min="12" max="12" width="5.68359375" customWidth="1"/>
+    <col min="13" max="13" width="10.47265625" bestFit="1"/>
+    <col min="14" max="14" width="18.15625" bestFit="1"/>
+    <col min="15" max="15" width="14.3125" bestFit="1"/>
+    <col min="16" max="16" width="39.68359375" bestFit="1"/>
+    <col min="17" max="17" width="67.47265625" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" customHeight="1">
+    <row r="1" spans="1:17" ht="15.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1199,11 +1001,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q2" t="str">
-        <f>_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2)</f>
+        <f t="shared" ref="Q2:Q33" si="1">_xlfn.CONCAT(P2,"_",B2,"_",D2,"_",E2)</f>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1254,11 +1056,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q3" t="str">
-        <f>_xlfn.CONCAT(P3,"_",B3,"_",D3,"_",E3)</f>
+        <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_population_1_1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1309,11 +1111,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q4" t="str">
-        <f>_xlfn.CONCAT(P4,"_",B4,"_",D4,"_",E4)</f>
+        <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_1_1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1364,11 +1166,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q5" t="str">
-        <f>_xlfn.CONCAT(P5,"_",B5,"_",D5,"_",E5)</f>
+        <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_shape_2_1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1419,11 +1221,11 @@
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q6" t="str">
-        <f>_xlfn.CONCAT(P6,"_",B6,"_",D6,"_",E6)</f>
+        <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021_survey_1_1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1474,11 +1276,11 @@
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q7" t="str">
-        <f>_xlfn.CONCAT(P7,"_",B7,"_",D7,"_",E7)</f>
+        <f t="shared" si="1"/>
         <v>mortality_survey_zzz_2021_dictionary_1_1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1529,11 +1331,11 @@
         <v>acutejaundicesyndrome_outbreak_tcd_2016</v>
       </c>
       <c r="Q8" t="str">
-        <f>_xlfn.CONCAT(P8,"_",B8,"_",D8,"_",E8)</f>
+        <f t="shared" si="1"/>
         <v>acutejaundicesyndrome_outbreak_tcd_2016_linelist_1_1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1584,11 +1386,11 @@
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q9" t="str">
-        <f>_xlfn.CONCAT(P9,"_",B9,"_",D9,"_",E9)</f>
+        <f t="shared" si="1"/>
         <v>covid-19_outbreak_usa_2020_linelist_1_1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1635,15 +1437,15 @@
         <v>28</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" ref="P10:P55" si="1">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
+        <f t="shared" ref="P10:P56" si="2">_xlfn.CONCAT(SUBSTITUTE(I10," ",""),"_",J10,"_",G10,"_",L10)</f>
         <v>covid-19_outbreak_usa_2020</v>
       </c>
       <c r="Q10" t="str">
-        <f>_xlfn.CONCAT(P10,"_",B10,"_",D10,"_",E10)</f>
+        <f t="shared" si="1"/>
         <v>covid-19_outbreak_usa_2020_linelist_1_2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1690,15 +1492,15 @@
         <v>28</v>
       </c>
       <c r="P11" t="str">
+        <f t="shared" si="2"/>
+        <v>covid-19_outbreak_usa_2020</v>
+      </c>
+      <c r="Q11" t="str">
         <f t="shared" si="1"/>
-        <v>covid-19_outbreak_usa_2020</v>
-      </c>
-      <c r="Q11" t="str">
-        <f>_xlfn.CONCAT(P11,"_",B11,"_",D11,"_",E11)</f>
         <v>covid-19_outbreak_usa_2020_population_1_1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1745,15 +1547,15 @@
         <v>28</v>
       </c>
       <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eue_2022</v>
+      </c>
+      <c r="Q12" t="str">
         <f t="shared" si="1"/>
-        <v>mpox_outbreak_eue_2022</v>
-      </c>
-      <c r="Q12" t="str">
-        <f>_xlfn.CONCAT(P12,"_",B12,"_",D12,"_",E12)</f>
         <v>mpox_outbreak_eue_2022_linelist_1_1</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1800,15 +1602,15 @@
         <v>28</v>
       </c>
       <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>mpox_outbreak_eue_2022</v>
+      </c>
+      <c r="Q13" t="str">
         <f t="shared" si="1"/>
-        <v>mpox_outbreak_eue_2022</v>
-      </c>
-      <c r="Q13" t="str">
-        <f>_xlfn.CONCAT(P13,"_",B13,"_",D13,"_",E13)</f>
         <v>mpox_outbreak_eue_2022_aggregate_1_1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1855,15 +1657,15 @@
         <v>28</v>
       </c>
       <c r="P14" t="str">
+        <f t="shared" si="2"/>
+        <v>salmonella_outbreak_deu_1998</v>
+      </c>
+      <c r="Q14" t="str">
         <f t="shared" si="1"/>
-        <v>salmonella_outbreak_deu_1998</v>
-      </c>
-      <c r="Q14" t="str">
-        <f>_xlfn.CONCAT(P14,"_",B14,"_",D14,"_",E14)</f>
         <v>salmonella_outbreak_deu_1998_linelist_1_1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1910,15 +1712,15 @@
         <v>79</v>
       </c>
       <c r="P15" t="str">
+        <f t="shared" si="2"/>
+        <v>influenza_outbreak_chn_2013</v>
+      </c>
+      <c r="Q15" t="str">
         <f t="shared" si="1"/>
-        <v>influenza_outbreak_chn_2013</v>
-      </c>
-      <c r="Q15" t="str">
-        <f>_xlfn.CONCAT(P15,"_",B15,"_",D15,"_",E15)</f>
         <v>influenza_outbreak_chn_2013_linelist_1_1</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1965,15 +1767,15 @@
         <v>79</v>
       </c>
       <c r="P16" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q16" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q16" t="str">
-        <f>_xlfn.CONCAT(P16,"_",B16,"_",D16,"_",E16)</f>
         <v>ebola_outbreak_sle_2014_linelist_1_1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -2020,15 +1822,15 @@
         <v>79</v>
       </c>
       <c r="P17" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q17" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q17" t="str">
-        <f>_xlfn.CONCAT(P17,"_",B17,"_",D17,"_",E17)</f>
         <v>ebola_outbreak_sle_2014_linelist_1_2</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -2075,15 +1877,15 @@
         <v>79</v>
       </c>
       <c r="P18" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q18" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q18" t="str">
-        <f>_xlfn.CONCAT(P18,"_",B18,"_",D18,"_",E18)</f>
         <v>ebola_outbreak_sle_2014_linelist_1_3</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2130,15 +1932,15 @@
         <v>79</v>
       </c>
       <c r="P19" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q19" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q19" t="str">
-        <f>_xlfn.CONCAT(P19,"_",B19,"_",D19,"_",E19)</f>
         <v>ebola_outbreak_sle_2014_linelist_1_4</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -2185,15 +1987,15 @@
         <v>79</v>
       </c>
       <c r="P20" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q20" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q20" t="str">
-        <f>_xlfn.CONCAT(P20,"_",B20,"_",D20,"_",E20)</f>
         <v>ebola_outbreak_sle_2014_linelist_1_5</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2240,15 +2042,15 @@
         <v>79</v>
       </c>
       <c r="P21" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q21" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q21" t="str">
-        <f>_xlfn.CONCAT(P21,"_",B21,"_",D21,"_",E21)</f>
         <v>ebola_outbreak_sle_2014_dictionary_1_1</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2295,15 +2097,15 @@
         <v>96</v>
       </c>
       <c r="P22" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q22" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q22" t="str">
-        <f>_xlfn.CONCAT(P22,"_",B22,"_",D22,"_",E22)</f>
         <v>ebola_outbreak_sle_2014_shape_1_1</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -2350,15 +2152,15 @@
         <v>96</v>
       </c>
       <c r="P23" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2020</v>
+      </c>
+      <c r="Q23" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2020</v>
-      </c>
-      <c r="Q23" t="str">
-        <f>_xlfn.CONCAT(P23,"_",B23,"_",D23,"_",E23)</f>
         <v>ebola_outbreak_sle_2020_population_1_1</v>
       </c>
     </row>
-    <row r="24" ht="15.75">
+    <row r="24" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
@@ -2405,15 +2207,15 @@
         <v>79</v>
       </c>
       <c r="P24" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q24" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q24" t="str">
-        <f>_xlfn.CONCAT(P24,"_",B24,"_",D24,"_",E24)</f>
         <v>ebola_outbreak_sle_2014_other_1_1</v>
       </c>
     </row>
-    <row r="25" ht="15.75">
+    <row r="25" spans="1:17" ht="14.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
@@ -2460,15 +2262,15 @@
         <v>79</v>
       </c>
       <c r="P25" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q25" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q25" t="str">
-        <f>_xlfn.CONCAT(P25,"_",B25,"_",D25,"_",E25)</f>
         <v>ebola_outbreak_sle_2014_other_2_1</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -2515,15 +2317,15 @@
         <v>79</v>
       </c>
       <c r="P26" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q26" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q26" t="str">
-        <f>_xlfn.CONCAT(P26,"_",B26,"_",D26,"_",E26)</f>
         <v>ebola_outbreak_sle_2014_other_3_1</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -2570,15 +2372,15 @@
         <v>79</v>
       </c>
       <c r="P27" t="str">
+        <f t="shared" si="2"/>
+        <v>ebola_outbreak_sle_2014</v>
+      </c>
+      <c r="Q27" t="str">
         <f t="shared" si="1"/>
-        <v>ebola_outbreak_sle_2014</v>
-      </c>
-      <c r="Q27" t="str">
-        <f>_xlfn.CONCAT(P27,"_",B27,"_",D27,"_",E27)</f>
         <v>ebola_outbreak_sle_2014_other_4_1</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2625,15 +2427,15 @@
         <v>44</v>
       </c>
       <c r="P28" t="str">
+        <f t="shared" si="2"/>
+        <v>contacttracing_outbreak_zzz_2020</v>
+      </c>
+      <c r="Q28" t="str">
         <f t="shared" si="1"/>
-        <v>contacttracing_outbreak_zzz_2020</v>
-      </c>
-      <c r="Q28" t="str">
-        <f>_xlfn.CONCAT(P28,"_",B28,"_",D28,"_",E28)</f>
         <v>contacttracing_outbreak_zzz_2020_linelist_1_1</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -2680,15 +2482,15 @@
         <v>44</v>
       </c>
       <c r="P29" t="str">
+        <f t="shared" si="2"/>
+        <v>contacttracing_outbreak_zzz_2020</v>
+      </c>
+      <c r="Q29" t="str">
         <f t="shared" si="1"/>
-        <v>contacttracing_outbreak_zzz_2020</v>
-      </c>
-      <c r="Q29" t="str">
-        <f>_xlfn.CONCAT(P29,"_",B29,"_",D29,"_",E29)</f>
         <v>contacttracing_outbreak_zzz_2020_linelist_2_1</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2735,15 +2537,15 @@
         <v>44</v>
       </c>
       <c r="P30" t="str">
+        <f t="shared" si="2"/>
+        <v>contacttracing_outbreak_zzz_2020</v>
+      </c>
+      <c r="Q30" t="str">
         <f t="shared" si="1"/>
-        <v>contacttracing_outbreak_zzz_2020</v>
-      </c>
-      <c r="Q30" t="str">
-        <f>_xlfn.CONCAT(P30,"_",B30,"_",D30,"_",E30)</f>
         <v>contacttracing_outbreak_zzz_2020_linelist_3_1</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2790,15 +2592,15 @@
         <v>44</v>
       </c>
       <c r="P31" t="str">
+        <f t="shared" si="2"/>
+        <v>contacttracing_outbreak_zzz_2020</v>
+      </c>
+      <c r="Q31" t="str">
         <f t="shared" si="1"/>
-        <v>contacttracing_outbreak_zzz_2020</v>
-      </c>
-      <c r="Q31" t="str">
-        <f>_xlfn.CONCAT(P31,"_",B31,"_",D31,"_",E31)</f>
         <v>contacttracing_outbreak_zzz_2020_linelist_4_1</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2845,15 +2647,15 @@
         <v>28</v>
       </c>
       <c r="P32" t="str">
+        <f t="shared" si="2"/>
+        <v>malaria_outbreak_moz_2019</v>
+      </c>
+      <c r="Q32" t="str">
         <f t="shared" si="1"/>
-        <v>malaria_outbreak_moz_2019</v>
-      </c>
-      <c r="Q32" t="str">
-        <f>_xlfn.CONCAT(P32,"_",B32,"_",D32,"_",E32)</f>
         <v>malaria_outbreak_moz_2019_aggregate_1_1</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2900,15 +2702,15 @@
         <v>28</v>
       </c>
       <c r="P33" t="str">
+        <f t="shared" si="2"/>
+        <v>malaria_outbreak_moz_2019</v>
+      </c>
+      <c r="Q33" t="str">
         <f t="shared" si="1"/>
-        <v>malaria_outbreak_moz_2019</v>
-      </c>
-      <c r="Q33" t="str">
-        <f>_xlfn.CONCAT(P33,"_",B33,"_",D33,"_",E33)</f>
         <v>malaria_outbreak_moz_2019_aggregate_1_2</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -2955,15 +2757,15 @@
         <v>28</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q34" t="str">
-        <f>_xlfn.CONCAT(P34,"_",B34,"_",D34,"_",E34)</f>
+        <f t="shared" ref="Q34:Q65" si="3">_xlfn.CONCAT(P34,"_",B34,"_",D34,"_",E34)</f>
         <v>shigella_surveillance_bel_2013_sequencing_1_1</v>
       </c>
     </row>
-    <row r="35" ht="15.5" customHeight="1">
+    <row r="35" spans="1:17" ht="15.55" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -3010,15 +2812,15 @@
         <v>28</v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q35" t="str">
-        <f>_xlfn.CONCAT(P35,"_",B35,"_",D35,"_",E35)</f>
+        <f t="shared" si="3"/>
         <v>shigella_surveillance_bel_2013_linelist_1_1</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>126</v>
       </c>
@@ -3065,15 +2867,15 @@
         <v>28</v>
       </c>
       <c r="P36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>shigella_surveillance_bel_2013</v>
       </c>
       <c r="Q36" t="str">
-        <f>_xlfn.CONCAT(P36,"_",B36,"_",D36,"_",E36)</f>
+        <f t="shared" si="3"/>
         <v>shigella_surveillance_bel_2013_sequencing_1_2</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -3120,15 +2922,15 @@
         <v>28</v>
       </c>
       <c r="P37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q37" t="str">
-        <f>_xlfn.CONCAT(P37,"_",B37,"_",D37,"_",E37)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_1_1</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -3175,15 +2977,15 @@
         <v>28</v>
       </c>
       <c r="P38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q38" t="str">
-        <f>_xlfn.CONCAT(P38,"_",B38,"_",D38,"_",E38)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_2_1</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -3230,15 +3032,15 @@
         <v>28</v>
       </c>
       <c r="P39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q39" t="str">
-        <f>_xlfn.CONCAT(P39,"_",B39,"_",D39,"_",E39)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_3_1</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -3285,15 +3087,15 @@
         <v>28</v>
       </c>
       <c r="P40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q40" t="str">
-        <f>_xlfn.CONCAT(P40,"_",B40,"_",D40,"_",E40)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_4_1</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3340,15 +3142,15 @@
         <v>135</v>
       </c>
       <c r="P41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_surveillance_zzz_2020</v>
       </c>
       <c r="Q41" t="str">
-        <f>_xlfn.CONCAT(P41,"_",B41,"_",D41,"_",E41)</f>
+        <f t="shared" si="3"/>
         <v>mortality_surveillance_zzz_2020_aggregate_5_1</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -3395,15 +3197,15 @@
         <v>28</v>
       </c>
       <c r="P42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>likert_other_zzz_2020</v>
       </c>
       <c r="Q42" t="str">
-        <f>_xlfn.CONCAT(P42,"_",B42,"_",D42,"_",E42)</f>
+        <f t="shared" si="3"/>
         <v>likert_other_zzz_2020_aggregate_1_1</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3450,15 +3252,15 @@
         <v>44</v>
       </c>
       <c r="P43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q43" t="str">
-        <f>_xlfn.CONCAT(P43,"_",B43,"_",D43,"_",E43)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_survey_2_1</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3505,15 +3307,15 @@
         <v>44</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q44" t="str">
-        <f>_xlfn.CONCAT(P44,"_",B44,"_",D44,"_",E44)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_dictionary_2_1</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -3560,15 +3362,15 @@
         <v>44</v>
       </c>
       <c r="P45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>mortality_survey_zzz_2021</v>
       </c>
       <c r="Q45" t="str">
-        <f>_xlfn.CONCAT(P45,"_",B45,"_",D45,"_",E45)</f>
+        <f t="shared" si="3"/>
         <v>mortality_survey_zzz_2021_population_1_1</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>144</v>
       </c>
@@ -3615,15 +3417,15 @@
         <v>44</v>
       </c>
       <c r="P46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>campylobacter_surveillance_deu_2001</v>
       </c>
       <c r="Q46" t="str">
-        <f>_xlfn.CONCAT(P46,"_",B46,"_",D46,"_",E46)</f>
+        <f t="shared" si="3"/>
         <v>campylobacter_surveillance_deu_2001_linelist_1_1</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>147</v>
       </c>
@@ -3670,22 +3472,22 @@
         <v>44</v>
       </c>
       <c r="P47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>weather_other_deu_2001</v>
       </c>
       <c r="Q47" t="str">
-        <f>_xlfn.CONCAT(P47,"_",B47,"_",D47,"_",E47)</f>
+        <f t="shared" si="3"/>
         <v>weather_other_deu_2001_aggregate_1_1</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" t="s">
         <v>67</v>
       </c>
       <c r="D48">
@@ -3694,28 +3496,28 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" s="4" t="s">
+      <c r="F48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" t="s">
         <v>40</v>
       </c>
       <c r="H48" t="s">
         <v>75</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" t="s">
         <v>151</v>
       </c>
       <c r="J48" t="s">
         <v>122</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" t="s">
         <v>42</v>
       </c>
       <c r="L48">
         <v>2024</v>
       </c>
-      <c r="M48" s="4" t="s">
+      <c r="M48" t="s">
         <v>152</v>
       </c>
       <c r="N48" t="s">
@@ -3725,22 +3527,22 @@
         <v>28</v>
       </c>
       <c r="P48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q48" t="str">
-        <f>_xlfn.CONCAT(P48,"_",B48,"_",D48,"_",E48)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
         <v>153</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49">
@@ -3749,28 +3551,28 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="4" t="s">
+      <c r="F49" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" t="s">
         <v>40</v>
       </c>
       <c r="H49" t="s">
         <v>75</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I49" t="s">
         <v>151</v>
       </c>
       <c r="J49" t="s">
         <v>122</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K49" t="s">
         <v>42</v>
       </c>
       <c r="L49">
         <v>2024</v>
       </c>
-      <c r="M49" s="4" t="s">
+      <c r="M49" t="s">
         <v>154</v>
       </c>
       <c r="N49" t="s">
@@ -3780,22 +3582,22 @@
         <v>28</v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q49" t="str">
-        <f>_xlfn.CONCAT(P49,"_",B49,"_",D49,"_",E49)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>155</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="D50">
@@ -3804,28 +3606,28 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" t="s">
         <v>49</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="G50" t="s">
         <v>40</v>
       </c>
       <c r="H50" t="s">
         <v>75</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" t="s">
         <v>151</v>
       </c>
       <c r="J50" t="s">
         <v>122</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" t="s">
         <v>42</v>
       </c>
       <c r="L50">
         <v>2024</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" t="s">
         <v>154</v>
       </c>
       <c r="N50" t="s">
@@ -3835,22 +3637,22 @@
         <v>28</v>
       </c>
       <c r="P50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q50" t="str">
-        <f>_xlfn.CONCAT(P50,"_",B50,"_",D50,"_",E50)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" t="s">
         <v>67</v>
       </c>
       <c r="D51">
@@ -3859,28 +3661,28 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" t="s">
         <v>49</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="G51" t="s">
         <v>40</v>
       </c>
       <c r="H51" t="s">
         <v>75</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I51" t="s">
         <v>151</v>
       </c>
       <c r="J51" t="s">
         <v>122</v>
       </c>
-      <c r="K51" s="4" t="s">
+      <c r="K51" t="s">
         <v>42</v>
       </c>
       <c r="L51">
         <v>2024</v>
       </c>
-      <c r="M51" s="4" t="s">
+      <c r="M51" t="s">
         <v>152</v>
       </c>
       <c r="N51" t="s">
@@ -3890,22 +3692,22 @@
         <v>28</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q51" t="str">
-        <f>_xlfn.CONCAT(P51,"_",B51,"_",D51,"_",E51)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>157</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>19</v>
       </c>
       <c r="D52">
@@ -3914,28 +3716,28 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" t="s">
         <v>158</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="G52" t="s">
         <v>40</v>
       </c>
       <c r="H52" t="s">
         <v>75</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="I52" t="s">
         <v>151</v>
       </c>
       <c r="J52" t="s">
         <v>122</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="K52" t="s">
         <v>42</v>
       </c>
       <c r="L52">
         <v>2024</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="M52" t="s">
         <v>154</v>
       </c>
       <c r="N52" t="s">
@@ -3945,22 +3747,22 @@
         <v>28</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q52" t="str">
-        <f>_xlfn.CONCAT(P52,"_",B52,"_",D52,"_",E52)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" t="s">
         <v>67</v>
       </c>
       <c r="D53">
@@ -3969,28 +3771,28 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" t="s">
         <v>158</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="G53" t="s">
         <v>40</v>
       </c>
       <c r="H53" t="s">
         <v>75</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I53" t="s">
         <v>151</v>
       </c>
       <c r="J53" t="s">
         <v>122</v>
       </c>
-      <c r="K53" s="4" t="s">
+      <c r="K53" t="s">
         <v>42</v>
       </c>
       <c r="L53">
         <v>2024</v>
       </c>
-      <c r="M53" s="4" t="s">
+      <c r="M53" t="s">
         <v>152</v>
       </c>
       <c r="N53" t="s">
@@ -4000,22 +3802,22 @@
         <v>28</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q53" t="str">
-        <f>_xlfn.CONCAT(P53,"_",B53,"_",D53,"_",E53)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>19</v>
       </c>
       <c r="D54">
@@ -4024,28 +3826,28 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" t="s">
         <v>161</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G54" t="s">
         <v>40</v>
       </c>
       <c r="H54" t="s">
         <v>75</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I54" t="s">
         <v>151</v>
       </c>
       <c r="J54" t="s">
         <v>122</v>
       </c>
-      <c r="K54" s="4" t="s">
+      <c r="K54" t="s">
         <v>42</v>
       </c>
       <c r="L54">
         <v>2024</v>
       </c>
-      <c r="M54" s="4" t="s">
+      <c r="M54" t="s">
         <v>154</v>
       </c>
       <c r="N54" t="s">
@@ -4055,22 +3857,22 @@
         <v>28</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q54" t="str">
-        <f>_xlfn.CONCAT(P54,"_",B54,"_",D54,"_",E54)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_2_1</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>67</v>
       </c>
       <c r="D55">
@@ -4079,28 +3881,28 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" t="s">
         <v>161</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G55" t="s">
         <v>40</v>
       </c>
       <c r="H55" t="s">
         <v>75</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" t="s">
         <v>151</v>
       </c>
       <c r="J55" t="s">
         <v>122</v>
       </c>
-      <c r="K55" s="4" t="s">
+      <c r="K55" t="s">
         <v>42</v>
       </c>
       <c r="L55">
         <v>2024</v>
       </c>
-      <c r="M55" s="4" t="s">
+      <c r="M55" t="s">
         <v>152</v>
       </c>
       <c r="N55" t="s">
@@ -4110,70 +3912,302 @@
         <v>28</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>multidisease_surveillance_zzz_2024</v>
       </c>
       <c r="Q55" t="str">
-        <f>_xlfn.CONCAT(P55,"_",B55,"_",D55,"_",E55)</f>
+        <f t="shared" si="3"/>
         <v>multidisease_surveillance_zzz_2024_linelist_1_1</v>
       </c>
     </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>171</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I56" t="s">
+        <v>163</v>
+      </c>
+      <c r="J56" t="s">
+        <v>122</v>
+      </c>
+      <c r="K56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L56">
+        <v>2021</v>
+      </c>
+      <c r="M56" t="s">
+        <v>166</v>
+      </c>
+      <c r="N56" t="s">
+        <v>165</v>
+      </c>
+      <c r="O56" t="s">
+        <v>28</v>
+      </c>
+      <c r="P56" t="str">
+        <f t="shared" si="2"/>
+        <v>cholera_surveillance_zzz_2021</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="3"/>
+        <v>cholera_surveillance_zzz_2021_linelist_1_1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" t="s">
+        <v>75</v>
+      </c>
+      <c r="I57" t="s">
+        <v>163</v>
+      </c>
+      <c r="J57" t="s">
+        <v>122</v>
+      </c>
+      <c r="K57" t="s">
+        <v>42</v>
+      </c>
+      <c r="L57">
+        <v>2021</v>
+      </c>
+      <c r="M57" t="s">
+        <v>164</v>
+      </c>
+      <c r="N57" t="s">
+        <v>165</v>
+      </c>
+      <c r="O57" t="s">
+        <v>28</v>
+      </c>
+      <c r="P57" t="str">
+        <f t="shared" ref="P57:P58" si="4">_xlfn.CONCAT(SUBSTITUTE(I57," ",""),"_",J57,"_",G57,"_",L57)</f>
+        <v>cholera_surveillance_zzz_2021</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" ref="Q57:Q58" si="5">_xlfn.CONCAT(P57,"_",B57,"_",D57,"_",E57)</f>
+        <v>cholera_surveillance_zzz_2021_linelist_1_2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" t="s">
+        <v>75</v>
+      </c>
+      <c r="I58" t="s">
+        <v>163</v>
+      </c>
+      <c r="J58" t="s">
+        <v>122</v>
+      </c>
+      <c r="K58" t="s">
+        <v>42</v>
+      </c>
+      <c r="L58">
+        <v>2021</v>
+      </c>
+      <c r="M58" t="s">
+        <v>167</v>
+      </c>
+      <c r="N58" t="s">
+        <v>165</v>
+      </c>
+      <c r="O58" t="s">
+        <v>28</v>
+      </c>
+      <c r="P58" t="str">
+        <f t="shared" si="4"/>
+        <v>cholera_surveillance_zzz_2021</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="5"/>
+        <v>cholera_surveillance_zzz_2021_linelist_1_3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" t="s">
+        <v>75</v>
+      </c>
+      <c r="I59" t="s">
+        <v>163</v>
+      </c>
+      <c r="J59" t="s">
+        <v>122</v>
+      </c>
+      <c r="K59" t="s">
+        <v>42</v>
+      </c>
+      <c r="L59">
+        <v>2021</v>
+      </c>
+      <c r="M59" t="s">
+        <v>168</v>
+      </c>
+      <c r="N59" t="s">
+        <v>165</v>
+      </c>
+      <c r="O59" t="s">
+        <v>28</v>
+      </c>
+      <c r="P59" t="str">
+        <f t="shared" ref="P59" si="6">_xlfn.CONCAT(SUBSTITUTE(I59," ",""),"_",J59,"_",G59,"_",L59)</f>
+        <v>cholera_surveillance_zzz_2021</v>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" ref="Q59" si="7">_xlfn.CONCAT(P59,"_",B59,"_",D59,"_",E59)</f>
+        <v>cholera_surveillance_zzz_2021_linelist_2_3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" t="s">
+        <v>40</v>
+      </c>
+      <c r="H60" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" t="s">
+        <v>163</v>
+      </c>
+      <c r="J60" t="s">
+        <v>122</v>
+      </c>
+      <c r="K60" t="s">
+        <v>42</v>
+      </c>
+      <c r="L60">
+        <v>2021</v>
+      </c>
+      <c r="M60" t="s">
+        <v>169</v>
+      </c>
+      <c r="N60" t="s">
+        <v>165</v>
+      </c>
+      <c r="O60" t="s">
+        <v>28</v>
+      </c>
+      <c r="P60" t="str">
+        <f t="shared" ref="P60" si="8">_xlfn.CONCAT(SUBSTITUTE(I60," ",""),"_",J60,"_",G60,"_",L60)</f>
+        <v>cholera_surveillance_zzz_2021</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" ref="Q60" si="9">_xlfn.CONCAT(P60,"_",B60,"_",D60,"_",E60)</f>
+        <v>cholera_surveillance_zzz_2021_linelist_3_3</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="3" id="{0074009D-0046-4C59-99FD-00C2004D0079}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:A53 A56:A1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="4" id="{00CB0073-008D-4E61-B735-005C00830098}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00AF0095-00BF-4E5C-A5A2-004D00880094}">
-            <xm:f>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor indexed="2"/>
-                  <bgColor indexed="2"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G2:G300</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
+  <conditionalFormatting sqref="A1:A53 A56:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G300 K56:K60">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(LEN(G2)&lt;&gt;3,LEN(G2)&lt;&gt;0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>